<commit_message>
correção da orientação em andamento e concluida de IC
</commit_message>
<xml_diff>
--- a/Planilha geral.xlsx
+++ b/Planilha geral.xlsx
@@ -522,45 +522,45 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -926,8 +926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:O160"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -967,12 +967,12 @@
       </c>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="61" t="s">
+      <c r="A4" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="61"/>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
+      <c r="B4" s="77"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="77"/>
       <c r="E4" s="48">
         <v>10</v>
       </c>
@@ -984,216 +984,216 @@
       </c>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="62" t="s">
+      <c r="A5" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="62"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="78"/>
       <c r="E5" s="48">
         <v>15</v>
       </c>
       <c r="F5" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="64" t="s">
+      <c r="J5" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="K5" s="64"/>
-      <c r="L5" s="64"/>
-      <c r="M5" s="64"/>
+      <c r="K5" s="61"/>
+      <c r="L5" s="61"/>
+      <c r="M5" s="61"/>
       <c r="N5" s="12" t="s">
         <v>25</v>
       </c>
       <c r="O5" s="23"/>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="62" t="s">
+      <c r="A6" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="62"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="78"/>
       <c r="E6" s="48">
         <v>8</v>
       </c>
       <c r="F6" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="J6" s="65" t="s">
+      <c r="J6" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="K6" s="65"/>
-      <c r="L6" s="65"/>
-      <c r="M6" s="65"/>
+      <c r="K6" s="62"/>
+      <c r="L6" s="62"/>
+      <c r="M6" s="62"/>
       <c r="N6" s="14" t="s">
         <v>27</v>
       </c>
       <c r="O6" s="23"/>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" s="61" t="s">
+      <c r="A7" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="61"/>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
+      <c r="B7" s="77"/>
+      <c r="C7" s="77"/>
+      <c r="D7" s="77"/>
       <c r="E7" s="48">
         <v>20</v>
       </c>
       <c r="F7" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="J7" s="78" t="s">
+      <c r="J7" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="78"/>
-      <c r="L7" s="78"/>
-      <c r="M7" s="78"/>
+      <c r="K7" s="63"/>
+      <c r="L7" s="63"/>
+      <c r="M7" s="63"/>
       <c r="N7" s="4">
         <v>5</v>
       </c>
       <c r="O7" s="2"/>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="61" t="s">
+      <c r="A8" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="61"/>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
+      <c r="B8" s="77"/>
+      <c r="C8" s="77"/>
+      <c r="D8" s="77"/>
       <c r="E8" s="48">
         <v>10</v>
       </c>
       <c r="F8" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="J8" s="78" t="s">
+      <c r="J8" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="78"/>
-      <c r="L8" s="78"/>
-      <c r="M8" s="78"/>
+      <c r="K8" s="63"/>
+      <c r="L8" s="63"/>
+      <c r="M8" s="63"/>
       <c r="N8" s="4">
         <v>10</v>
       </c>
       <c r="O8" s="2"/>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="61" t="s">
+      <c r="A9" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="61"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
+      <c r="B9" s="77"/>
+      <c r="C9" s="77"/>
+      <c r="D9" s="77"/>
       <c r="E9" s="48">
         <v>5</v>
       </c>
       <c r="F9" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="J9" s="78" t="s">
+      <c r="J9" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="78"/>
-      <c r="L9" s="78"/>
-      <c r="M9" s="78"/>
+      <c r="K9" s="63"/>
+      <c r="L9" s="63"/>
+      <c r="M9" s="63"/>
       <c r="N9" s="4">
         <v>10</v>
       </c>
       <c r="O9" s="2"/>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10" s="62" t="s">
+      <c r="A10" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="62"/>
-      <c r="C10" s="62"/>
-      <c r="D10" s="62"/>
+      <c r="B10" s="78"/>
+      <c r="C10" s="78"/>
+      <c r="D10" s="78"/>
       <c r="E10" s="48">
         <v>3</v>
       </c>
       <c r="F10" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="J10" s="78" t="s">
+      <c r="J10" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="K10" s="78"/>
-      <c r="L10" s="78"/>
-      <c r="M10" s="78"/>
+      <c r="K10" s="63"/>
+      <c r="L10" s="63"/>
+      <c r="M10" s="63"/>
       <c r="N10" s="4">
         <v>15</v>
       </c>
       <c r="O10" s="2"/>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11" s="58" t="s">
+      <c r="A11" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="58"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58"/>
+      <c r="B11" s="75"/>
+      <c r="C11" s="75"/>
+      <c r="D11" s="75"/>
       <c r="E11" s="48">
         <v>10</v>
       </c>
       <c r="F11" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="J11" s="68" t="s">
+      <c r="J11" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="K11" s="68"/>
-      <c r="L11" s="68"/>
-      <c r="M11" s="68"/>
+      <c r="K11" s="64"/>
+      <c r="L11" s="64"/>
+      <c r="M11" s="64"/>
     </row>
     <row r="12" spans="1:15">
-      <c r="A12" s="58" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="58"/>
-      <c r="C12" s="58"/>
-      <c r="D12" s="58"/>
+      <c r="A12" s="75" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="75"/>
+      <c r="C12" s="75"/>
+      <c r="D12" s="75"/>
       <c r="E12" s="48">
         <v>15</v>
       </c>
       <c r="F12" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="J12" s="68" t="s">
+      <c r="J12" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="K12" s="68"/>
-      <c r="L12" s="68"/>
-      <c r="M12" s="68"/>
+      <c r="K12" s="64"/>
+      <c r="L12" s="64"/>
+      <c r="M12" s="64"/>
     </row>
     <row r="13" spans="1:15">
-      <c r="A13" s="59" t="s">
+      <c r="A13" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="59"/>
-      <c r="C13" s="59"/>
-      <c r="D13" s="59"/>
+      <c r="B13" s="76"/>
+      <c r="C13" s="76"/>
+      <c r="D13" s="76"/>
       <c r="E13" s="49">
         <v>5</v>
       </c>
       <c r="F13" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="J13" s="69" t="s">
+      <c r="J13" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="69"/>
-      <c r="L13" s="69"/>
-      <c r="M13" s="69"/>
+      <c r="K13" s="65"/>
+      <c r="L13" s="65"/>
+      <c r="M13" s="65"/>
     </row>
     <row r="14" spans="1:15">
-      <c r="A14" s="59" t="s">
+      <c r="A14" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="59"/>
-      <c r="C14" s="59"/>
-      <c r="D14" s="59"/>
+      <c r="B14" s="76"/>
+      <c r="C14" s="76"/>
+      <c r="D14" s="76"/>
       <c r="E14" s="49">
         <v>7</v>
       </c>
@@ -1350,12 +1350,12 @@
       <c r="D22" s="60"/>
       <c r="E22" s="60"/>
       <c r="F22" s="60"/>
-      <c r="J22" s="73" t="s">
+      <c r="J22" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="K22" s="73"/>
-      <c r="L22" s="73"/>
-      <c r="M22" s="73"/>
+      <c r="K22" s="58"/>
+      <c r="L22" s="58"/>
+      <c r="M22" s="58"/>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="39" t="s">
@@ -1372,12 +1372,12 @@
       </c>
     </row>
     <row r="24" spans="1:13">
-      <c r="A24" s="63" t="s">
+      <c r="A24" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="63"/>
-      <c r="C24" s="63"/>
-      <c r="D24" s="63"/>
+      <c r="B24" s="72"/>
+      <c r="C24" s="72"/>
+      <c r="D24" s="72"/>
       <c r="E24" s="10">
         <v>10</v>
       </c>
@@ -1386,36 +1386,36 @@
       </c>
     </row>
     <row r="25" spans="1:13">
-      <c r="A25" s="64" t="s">
+      <c r="A25" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="64"/>
-      <c r="C25" s="64"/>
-      <c r="D25" s="64"/>
+      <c r="B25" s="61"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="61"/>
       <c r="E25" s="12" t="s">
         <v>25</v>
       </c>
       <c r="F25" s="13"/>
     </row>
     <row r="26" spans="1:13">
-      <c r="A26" s="65" t="s">
+      <c r="A26" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="65"/>
-      <c r="C26" s="65"/>
-      <c r="D26" s="65"/>
+      <c r="B26" s="62"/>
+      <c r="C26" s="62"/>
+      <c r="D26" s="62"/>
       <c r="E26" s="14" t="s">
         <v>27</v>
       </c>
       <c r="F26" s="13"/>
     </row>
     <row r="27" spans="1:13">
-      <c r="A27" s="63" t="s">
+      <c r="A27" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="63"/>
-      <c r="C27" s="63"/>
-      <c r="D27" s="63"/>
+      <c r="B27" s="72"/>
+      <c r="C27" s="72"/>
+      <c r="D27" s="72"/>
       <c r="E27" s="10">
         <v>15</v>
       </c>
@@ -1424,12 +1424,12 @@
       </c>
     </row>
     <row r="28" spans="1:13">
-      <c r="A28" s="63" t="s">
+      <c r="A28" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="63"/>
-      <c r="C28" s="63"/>
-      <c r="D28" s="63"/>
+      <c r="B28" s="72"/>
+      <c r="C28" s="72"/>
+      <c r="D28" s="72"/>
       <c r="E28" s="10">
         <v>10</v>
       </c>
@@ -1438,12 +1438,12 @@
       </c>
     </row>
     <row r="29" spans="1:13">
-      <c r="A29" s="66" t="s">
+      <c r="A29" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="66"/>
-      <c r="C29" s="66"/>
-      <c r="D29" s="66"/>
+      <c r="B29" s="73"/>
+      <c r="C29" s="73"/>
+      <c r="D29" s="73"/>
       <c r="E29" s="10">
         <v>10</v>
       </c>
@@ -1453,12 +1453,12 @@
       <c r="M29" s="57"/>
     </row>
     <row r="30" spans="1:13">
-      <c r="A30" s="66" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" s="66"/>
-      <c r="C30" s="66"/>
-      <c r="D30" s="66"/>
+      <c r="A30" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="73"/>
+      <c r="C30" s="73"/>
+      <c r="D30" s="73"/>
       <c r="E30" s="10">
         <v>15</v>
       </c>
@@ -1467,12 +1467,12 @@
       </c>
     </row>
     <row r="31" spans="1:13">
-      <c r="A31" s="67" t="s">
+      <c r="A31" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="67"/>
-      <c r="C31" s="67"/>
-      <c r="D31" s="67"/>
+      <c r="B31" s="74"/>
+      <c r="C31" s="74"/>
+      <c r="D31" s="74"/>
       <c r="E31" s="11">
         <v>5</v>
       </c>
@@ -1481,12 +1481,12 @@
       </c>
     </row>
     <row r="32" spans="1:13">
-      <c r="A32" s="67" t="s">
+      <c r="A32" s="74" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="67"/>
-      <c r="C32" s="67"/>
-      <c r="D32" s="67"/>
+      <c r="B32" s="74"/>
+      <c r="C32" s="74"/>
+      <c r="D32" s="74"/>
       <c r="E32" s="11">
         <v>7</v>
       </c>
@@ -1610,12 +1610,12 @@
       </c>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="68" t="s">
+      <c r="A43" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B43" s="68"/>
-      <c r="C43" s="68"/>
-      <c r="D43" s="68"/>
+      <c r="B43" s="64"/>
+      <c r="C43" s="64"/>
+      <c r="D43" s="64"/>
       <c r="E43" s="25">
         <v>10</v>
       </c>
@@ -1627,12 +1627,12 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="68" t="s">
+      <c r="A44" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="B44" s="68"/>
-      <c r="C44" s="68"/>
-      <c r="D44" s="68"/>
+      <c r="B44" s="64"/>
+      <c r="C44" s="64"/>
+      <c r="D44" s="64"/>
       <c r="E44" s="25">
         <v>16</v>
       </c>
@@ -1642,12 +1642,12 @@
       <c r="G44" s="26"/>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="68" t="s">
+      <c r="A45" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="B45" s="68"/>
-      <c r="C45" s="68"/>
-      <c r="D45" s="68"/>
+      <c r="B45" s="64"/>
+      <c r="C45" s="64"/>
+      <c r="D45" s="64"/>
       <c r="E45" s="25">
         <v>10</v>
       </c>
@@ -1657,12 +1657,12 @@
       <c r="G45" s="26"/>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="69" t="s">
+      <c r="A46" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="B46" s="69"/>
-      <c r="C46" s="69"/>
-      <c r="D46" s="69"/>
+      <c r="B46" s="65"/>
+      <c r="C46" s="65"/>
+      <c r="D46" s="65"/>
       <c r="E46" s="25">
         <v>8</v>
       </c>
@@ -1687,12 +1687,12 @@
       <c r="G47" s="26"/>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="68" t="s">
+      <c r="A48" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="B48" s="68"/>
-      <c r="C48" s="68"/>
-      <c r="D48" s="68"/>
+      <c r="B48" s="64"/>
+      <c r="C48" s="64"/>
+      <c r="D48" s="64"/>
       <c r="E48" s="25">
         <v>15</v>
       </c>
@@ -1704,12 +1704,12 @@
       </c>
     </row>
     <row r="49" spans="1:7">
-      <c r="A49" s="68" t="s">
+      <c r="A49" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="B49" s="68"/>
-      <c r="C49" s="68"/>
-      <c r="D49" s="68"/>
+      <c r="B49" s="64"/>
+      <c r="C49" s="64"/>
+      <c r="D49" s="64"/>
       <c r="E49" s="25">
         <v>5</v>
       </c>
@@ -1721,12 +1721,12 @@
       </c>
     </row>
     <row r="50" spans="1:7">
-      <c r="A50" s="68" t="s">
+      <c r="A50" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="B50" s="68"/>
-      <c r="C50" s="68"/>
-      <c r="D50" s="68"/>
+      <c r="B50" s="64"/>
+      <c r="C50" s="64"/>
+      <c r="D50" s="64"/>
       <c r="E50" s="25">
         <v>0</v>
       </c>
@@ -1738,40 +1738,40 @@
       </c>
     </row>
     <row r="51" spans="1:7">
-      <c r="A51" s="69" t="s">
+      <c r="A51" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="B51" s="69"/>
-      <c r="C51" s="69"/>
-      <c r="D51" s="69"/>
+      <c r="B51" s="65"/>
+      <c r="C51" s="65"/>
+      <c r="D51" s="65"/>
       <c r="E51" s="25">
         <v>6</v>
       </c>
-      <c r="F51" s="70">
+      <c r="F51" s="71">
         <v>9</v>
       </c>
       <c r="G51" s="26"/>
     </row>
     <row r="52" spans="1:7">
-      <c r="A52" s="68" t="s">
+      <c r="A52" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="B52" s="68"/>
-      <c r="C52" s="68"/>
-      <c r="D52" s="68"/>
+      <c r="B52" s="64"/>
+      <c r="C52" s="64"/>
+      <c r="D52" s="64"/>
       <c r="E52" s="25">
         <v>4</v>
       </c>
-      <c r="F52" s="70"/>
+      <c r="F52" s="71"/>
       <c r="G52" s="26"/>
     </row>
     <row r="53" spans="1:7">
-      <c r="A53" s="69" t="s">
+      <c r="A53" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="B53" s="69"/>
-      <c r="C53" s="69"/>
-      <c r="D53" s="69"/>
+      <c r="B53" s="65"/>
+      <c r="C53" s="65"/>
+      <c r="D53" s="65"/>
       <c r="E53" s="25">
         <v>10</v>
       </c>
@@ -1783,12 +1783,12 @@
       </c>
     </row>
     <row r="54" spans="1:7">
-      <c r="A54" s="69" t="s">
-        <v>10</v>
-      </c>
-      <c r="B54" s="69"/>
-      <c r="C54" s="69"/>
-      <c r="D54" s="69"/>
+      <c r="A54" s="65" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" s="65"/>
+      <c r="C54" s="65"/>
+      <c r="D54" s="65"/>
       <c r="E54" s="25">
         <v>15</v>
       </c>
@@ -1800,12 +1800,12 @@
       </c>
     </row>
     <row r="55" spans="1:7">
-      <c r="A55" s="68" t="s">
+      <c r="A55" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="B55" s="68"/>
-      <c r="C55" s="68"/>
-      <c r="D55" s="68"/>
+      <c r="B55" s="64"/>
+      <c r="C55" s="64"/>
+      <c r="D55" s="64"/>
       <c r="E55" s="25">
         <v>1</v>
       </c>
@@ -1817,12 +1817,12 @@
       </c>
     </row>
     <row r="56" spans="1:7">
-      <c r="A56" s="68" t="s">
+      <c r="A56" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="B56" s="68"/>
-      <c r="C56" s="68"/>
-      <c r="D56" s="68"/>
+      <c r="B56" s="64"/>
+      <c r="C56" s="64"/>
+      <c r="D56" s="64"/>
       <c r="E56" s="25">
         <v>2</v>
       </c>
@@ -1834,12 +1834,12 @@
       </c>
     </row>
     <row r="57" spans="1:7">
-      <c r="A57" s="68" t="s">
+      <c r="A57" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B57" s="68"/>
-      <c r="C57" s="68"/>
-      <c r="D57" s="68"/>
+      <c r="B57" s="64"/>
+      <c r="C57" s="64"/>
+      <c r="D57" s="64"/>
       <c r="E57" s="25">
         <v>1.5</v>
       </c>
@@ -1885,12 +1885,12 @@
       </c>
     </row>
     <row r="60" spans="1:7">
-      <c r="A60" s="68" t="s">
+      <c r="A60" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="B60" s="68"/>
-      <c r="C60" s="68"/>
-      <c r="D60" s="68"/>
+      <c r="B60" s="64"/>
+      <c r="C60" s="64"/>
+      <c r="D60" s="64"/>
       <c r="E60" s="25">
         <v>10</v>
       </c>
@@ -1919,12 +1919,12 @@
       </c>
     </row>
     <row r="62" spans="1:7">
-      <c r="A62" s="71" t="s">
+      <c r="A62" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="B62" s="71"/>
-      <c r="C62" s="71"/>
-      <c r="D62" s="71"/>
+      <c r="B62" s="70"/>
+      <c r="C62" s="70"/>
+      <c r="D62" s="70"/>
       <c r="E62" s="25">
         <v>2</v>
       </c>
@@ -1953,12 +1953,12 @@
       </c>
     </row>
     <row r="64" spans="1:7">
-      <c r="A64" s="71" t="s">
+      <c r="A64" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="B64" s="71"/>
-      <c r="C64" s="71"/>
-      <c r="D64" s="71"/>
+      <c r="B64" s="70"/>
+      <c r="C64" s="70"/>
+      <c r="D64" s="70"/>
       <c r="E64" s="25">
         <v>0.5</v>
       </c>
@@ -1968,12 +1968,12 @@
       <c r="G64" s="26"/>
     </row>
     <row r="65" spans="1:7">
-      <c r="A65" s="71" t="s">
+      <c r="A65" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="B65" s="71"/>
-      <c r="C65" s="71"/>
-      <c r="D65" s="71"/>
+      <c r="B65" s="70"/>
+      <c r="C65" s="70"/>
+      <c r="D65" s="70"/>
       <c r="E65" s="25">
         <v>3</v>
       </c>
@@ -2009,12 +2009,12 @@
       </c>
     </row>
     <row r="70" spans="1:7">
-      <c r="A70" s="72" t="s">
+      <c r="A70" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="B70" s="72"/>
-      <c r="C70" s="72"/>
-      <c r="D70" s="72"/>
+      <c r="B70" s="68"/>
+      <c r="C70" s="68"/>
+      <c r="D70" s="68"/>
       <c r="E70" s="23">
         <v>10</v>
       </c>
@@ -2023,12 +2023,12 @@
       </c>
     </row>
     <row r="71" spans="1:7">
-      <c r="A71" s="73" t="s">
+      <c r="A71" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="B71" s="73"/>
-      <c r="C71" s="73"/>
-      <c r="D71" s="73"/>
+      <c r="B71" s="58"/>
+      <c r="C71" s="58"/>
+      <c r="D71" s="58"/>
       <c r="E71" s="23">
         <v>20</v>
       </c>
@@ -2037,12 +2037,12 @@
       </c>
     </row>
     <row r="72" spans="1:7">
-      <c r="A72" s="73" t="s">
+      <c r="A72" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="B72" s="73"/>
-      <c r="C72" s="73"/>
-      <c r="D72" s="73"/>
+      <c r="B72" s="58"/>
+      <c r="C72" s="58"/>
+      <c r="D72" s="58"/>
       <c r="E72" s="23">
         <v>10</v>
       </c>
@@ -2051,12 +2051,12 @@
       </c>
     </row>
     <row r="73" spans="1:7">
-      <c r="A73" s="72" t="s">
+      <c r="A73" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="B73" s="72"/>
-      <c r="C73" s="72"/>
-      <c r="D73" s="72"/>
+      <c r="B73" s="68"/>
+      <c r="C73" s="68"/>
+      <c r="D73" s="68"/>
       <c r="E73" s="23">
         <v>20</v>
       </c>
@@ -2065,12 +2065,12 @@
       </c>
     </row>
     <row r="74" spans="1:7">
-      <c r="A74" s="72" t="s">
+      <c r="A74" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="B74" s="72"/>
-      <c r="C74" s="72"/>
-      <c r="D74" s="72"/>
+      <c r="B74" s="68"/>
+      <c r="C74" s="68"/>
+      <c r="D74" s="68"/>
       <c r="E74" s="23">
         <v>15</v>
       </c>
@@ -2079,12 +2079,12 @@
       </c>
     </row>
     <row r="75" spans="1:7">
-      <c r="A75" s="72" t="s">
+      <c r="A75" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="B75" s="72"/>
-      <c r="C75" s="72"/>
-      <c r="D75" s="72"/>
+      <c r="B75" s="68"/>
+      <c r="C75" s="68"/>
+      <c r="D75" s="68"/>
       <c r="E75" s="23">
         <v>10</v>
       </c>
@@ -2093,12 +2093,12 @@
       </c>
     </row>
     <row r="76" spans="1:7">
-      <c r="A76" s="73" t="s">
+      <c r="A76" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="B76" s="73"/>
-      <c r="C76" s="73"/>
-      <c r="D76" s="73"/>
+      <c r="B76" s="58"/>
+      <c r="C76" s="58"/>
+      <c r="D76" s="58"/>
       <c r="E76" s="23">
         <v>5</v>
       </c>
@@ -2107,12 +2107,12 @@
       </c>
     </row>
     <row r="77" spans="1:7">
-      <c r="A77" s="74" t="s">
+      <c r="A77" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="B77" s="74"/>
-      <c r="C77" s="74"/>
-      <c r="D77" s="74"/>
+      <c r="B77" s="67"/>
+      <c r="C77" s="67"/>
+      <c r="D77" s="67"/>
       <c r="E77" s="23">
         <v>10</v>
       </c>
@@ -2121,12 +2121,12 @@
       </c>
     </row>
     <row r="78" spans="1:7">
-      <c r="A78" s="74" t="s">
-        <v>10</v>
-      </c>
-      <c r="B78" s="74"/>
-      <c r="C78" s="74"/>
-      <c r="D78" s="74"/>
+      <c r="A78" s="67" t="s">
+        <v>10</v>
+      </c>
+      <c r="B78" s="67"/>
+      <c r="C78" s="67"/>
+      <c r="D78" s="67"/>
       <c r="E78" s="23">
         <v>15</v>
       </c>
@@ -2135,12 +2135,12 @@
       </c>
     </row>
     <row r="79" spans="1:7">
-      <c r="A79" s="73" t="s">
+      <c r="A79" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="B79" s="73"/>
-      <c r="C79" s="73"/>
-      <c r="D79" s="73"/>
+      <c r="B79" s="58"/>
+      <c r="C79" s="58"/>
+      <c r="D79" s="58"/>
       <c r="E79" s="13">
         <v>5</v>
       </c>
@@ -2149,12 +2149,12 @@
       </c>
     </row>
     <row r="80" spans="1:7">
-      <c r="A80" s="73" t="s">
+      <c r="A80" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="B80" s="73"/>
-      <c r="C80" s="73"/>
-      <c r="D80" s="73"/>
+      <c r="B80" s="58"/>
+      <c r="C80" s="58"/>
+      <c r="D80" s="58"/>
       <c r="E80" s="13">
         <v>7</v>
       </c>
@@ -2271,12 +2271,12 @@
       </c>
     </row>
     <row r="91" spans="1:6">
-      <c r="A91" s="72" t="s">
+      <c r="A91" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="B91" s="72"/>
-      <c r="C91" s="72"/>
-      <c r="D91" s="72"/>
+      <c r="B91" s="68"/>
+      <c r="C91" s="68"/>
+      <c r="D91" s="68"/>
       <c r="E91" s="23">
         <v>10</v>
       </c>
@@ -2285,120 +2285,120 @@
       </c>
     </row>
     <row r="92" spans="1:6">
-      <c r="A92" s="75" t="s">
+      <c r="A92" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="B92" s="75"/>
-      <c r="C92" s="75"/>
-      <c r="D92" s="75"/>
+      <c r="B92" s="69"/>
+      <c r="C92" s="69"/>
+      <c r="D92" s="69"/>
       <c r="E92" s="23">
         <v>10</v>
       </c>
       <c r="F92" s="13"/>
     </row>
     <row r="93" spans="1:6">
-      <c r="A93" s="75" t="s">
+      <c r="A93" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="B93" s="75"/>
-      <c r="C93" s="75"/>
-      <c r="D93" s="75"/>
+      <c r="B93" s="69"/>
+      <c r="C93" s="69"/>
+      <c r="D93" s="69"/>
       <c r="E93" s="23">
         <v>15</v>
       </c>
       <c r="F93" s="13"/>
     </row>
     <row r="94" spans="1:6">
-      <c r="A94" s="75" t="s">
+      <c r="A94" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="B94" s="75"/>
-      <c r="C94" s="75"/>
-      <c r="D94" s="75"/>
+      <c r="B94" s="69"/>
+      <c r="C94" s="69"/>
+      <c r="D94" s="69"/>
       <c r="E94" s="23">
         <v>12</v>
       </c>
       <c r="F94" s="13"/>
     </row>
     <row r="95" spans="1:6">
-      <c r="A95" s="73" t="s">
+      <c r="A95" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="B95" s="73"/>
-      <c r="C95" s="73"/>
-      <c r="D95" s="73"/>
+      <c r="B95" s="58"/>
+      <c r="C95" s="58"/>
+      <c r="D95" s="58"/>
       <c r="E95" s="23">
         <v>8</v>
       </c>
       <c r="F95" s="13"/>
     </row>
     <row r="96" spans="1:6">
-      <c r="A96" s="73" t="s">
+      <c r="A96" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="B96" s="73"/>
-      <c r="C96" s="73"/>
-      <c r="D96" s="73"/>
+      <c r="B96" s="58"/>
+      <c r="C96" s="58"/>
+      <c r="D96" s="58"/>
       <c r="E96" s="23">
         <v>4</v>
       </c>
       <c r="F96" s="13"/>
     </row>
     <row r="97" spans="1:6">
-      <c r="A97" s="75" t="s">
+      <c r="A97" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="B97" s="75"/>
-      <c r="C97" s="75"/>
-      <c r="D97" s="75"/>
+      <c r="B97" s="69"/>
+      <c r="C97" s="69"/>
+      <c r="D97" s="69"/>
       <c r="E97" s="23">
         <v>7.5</v>
       </c>
       <c r="F97" s="13"/>
     </row>
     <row r="98" spans="1:6">
-      <c r="A98" s="75" t="s">
+      <c r="A98" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="B98" s="75"/>
-      <c r="C98" s="75"/>
-      <c r="D98" s="75"/>
+      <c r="B98" s="69"/>
+      <c r="C98" s="69"/>
+      <c r="D98" s="69"/>
       <c r="E98" s="23">
         <v>6</v>
       </c>
       <c r="F98" s="13"/>
     </row>
     <row r="99" spans="1:6">
-      <c r="A99" s="73" t="s">
+      <c r="A99" s="58" t="s">
         <v>52</v>
       </c>
-      <c r="B99" s="73"/>
-      <c r="C99" s="73"/>
-      <c r="D99" s="73"/>
+      <c r="B99" s="58"/>
+      <c r="C99" s="58"/>
+      <c r="D99" s="58"/>
       <c r="E99" s="23">
         <v>4</v>
       </c>
       <c r="F99" s="13"/>
     </row>
     <row r="100" spans="1:6">
-      <c r="A100" s="73" t="s">
+      <c r="A100" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="B100" s="73"/>
-      <c r="C100" s="73"/>
-      <c r="D100" s="73"/>
+      <c r="B100" s="58"/>
+      <c r="C100" s="58"/>
+      <c r="D100" s="58"/>
       <c r="E100" s="23">
         <v>2</v>
       </c>
       <c r="F100" s="13"/>
     </row>
     <row r="101" spans="1:6">
-      <c r="A101" s="72" t="s">
+      <c r="A101" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="B101" s="72"/>
-      <c r="C101" s="72"/>
-      <c r="D101" s="72"/>
+      <c r="B101" s="68"/>
+      <c r="C101" s="68"/>
+      <c r="D101" s="68"/>
       <c r="E101" s="23">
         <v>20</v>
       </c>
@@ -2407,12 +2407,12 @@
       </c>
     </row>
     <row r="102" spans="1:6">
-      <c r="A102" s="72" t="s">
+      <c r="A102" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="B102" s="72"/>
-      <c r="C102" s="72"/>
-      <c r="D102" s="72"/>
+      <c r="B102" s="68"/>
+      <c r="C102" s="68"/>
+      <c r="D102" s="68"/>
       <c r="E102" s="23">
         <v>15</v>
       </c>
@@ -2421,12 +2421,12 @@
       </c>
     </row>
     <row r="103" spans="1:6">
-      <c r="A103" s="72" t="s">
+      <c r="A103" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="B103" s="72"/>
-      <c r="C103" s="72"/>
-      <c r="D103" s="72"/>
+      <c r="B103" s="68"/>
+      <c r="C103" s="68"/>
+      <c r="D103" s="68"/>
       <c r="E103" s="23">
         <v>10</v>
       </c>
@@ -2435,12 +2435,12 @@
       </c>
     </row>
     <row r="104" spans="1:6">
-      <c r="A104" s="73" t="s">
+      <c r="A104" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="B104" s="73"/>
-      <c r="C104" s="73"/>
-      <c r="D104" s="73"/>
+      <c r="B104" s="58"/>
+      <c r="C104" s="58"/>
+      <c r="D104" s="58"/>
       <c r="E104" s="23">
         <v>5</v>
       </c>
@@ -2449,12 +2449,12 @@
       </c>
     </row>
     <row r="105" spans="1:6">
-      <c r="A105" s="74" t="s">
+      <c r="A105" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="B105" s="74"/>
-      <c r="C105" s="74"/>
-      <c r="D105" s="74"/>
+      <c r="B105" s="67"/>
+      <c r="C105" s="67"/>
+      <c r="D105" s="67"/>
       <c r="E105" s="23">
         <v>10</v>
       </c>
@@ -2463,12 +2463,12 @@
       </c>
     </row>
     <row r="106" spans="1:6">
-      <c r="A106" s="74" t="s">
-        <v>10</v>
-      </c>
-      <c r="B106" s="74"/>
-      <c r="C106" s="74"/>
-      <c r="D106" s="74"/>
+      <c r="A106" s="67" t="s">
+        <v>10</v>
+      </c>
+      <c r="B106" s="67"/>
+      <c r="C106" s="67"/>
+      <c r="D106" s="67"/>
       <c r="E106" s="23">
         <v>15</v>
       </c>
@@ -2477,12 +2477,12 @@
       </c>
     </row>
     <row r="107" spans="1:6">
-      <c r="A107" s="73" t="s">
+      <c r="A107" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="B107" s="73"/>
-      <c r="C107" s="73"/>
-      <c r="D107" s="73"/>
+      <c r="B107" s="58"/>
+      <c r="C107" s="58"/>
+      <c r="D107" s="58"/>
       <c r="E107" s="13">
         <v>5</v>
       </c>
@@ -2491,12 +2491,12 @@
       </c>
     </row>
     <row r="108" spans="1:6">
-      <c r="A108" s="73" t="s">
+      <c r="A108" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="B108" s="73"/>
-      <c r="C108" s="73"/>
-      <c r="D108" s="73"/>
+      <c r="B108" s="58"/>
+      <c r="C108" s="58"/>
+      <c r="D108" s="58"/>
       <c r="E108" s="13">
         <v>7</v>
       </c>
@@ -2613,12 +2613,12 @@
       </c>
     </row>
     <row r="119" spans="1:6">
-      <c r="A119" s="72" t="s">
+      <c r="A119" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="B119" s="72"/>
-      <c r="C119" s="72"/>
-      <c r="D119" s="72"/>
+      <c r="B119" s="68"/>
+      <c r="C119" s="68"/>
+      <c r="D119" s="68"/>
       <c r="E119" s="23">
         <v>10</v>
       </c>
@@ -2627,12 +2627,12 @@
       </c>
     </row>
     <row r="120" spans="1:6">
-      <c r="A120" s="73" t="s">
+      <c r="A120" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="B120" s="73"/>
-      <c r="C120" s="73"/>
-      <c r="D120" s="73"/>
+      <c r="B120" s="58"/>
+      <c r="C120" s="58"/>
+      <c r="D120" s="58"/>
       <c r="E120" s="23">
         <v>30</v>
       </c>
@@ -2641,12 +2641,12 @@
       </c>
     </row>
     <row r="121" spans="1:6">
-      <c r="A121" s="73" t="s">
+      <c r="A121" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="B121" s="73"/>
-      <c r="C121" s="73"/>
-      <c r="D121" s="73"/>
+      <c r="B121" s="58"/>
+      <c r="C121" s="58"/>
+      <c r="D121" s="58"/>
       <c r="E121" s="23">
         <v>15</v>
       </c>
@@ -2655,12 +2655,12 @@
       </c>
     </row>
     <row r="122" spans="1:6">
-      <c r="A122" s="72" t="s">
+      <c r="A122" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="B122" s="72"/>
-      <c r="C122" s="72"/>
-      <c r="D122" s="72"/>
+      <c r="B122" s="68"/>
+      <c r="C122" s="68"/>
+      <c r="D122" s="68"/>
       <c r="E122" s="23">
         <v>50</v>
       </c>
@@ -2669,12 +2669,12 @@
       </c>
     </row>
     <row r="123" spans="1:6">
-      <c r="A123" s="72" t="s">
+      <c r="A123" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="B123" s="72"/>
-      <c r="C123" s="72"/>
-      <c r="D123" s="72"/>
+      <c r="B123" s="68"/>
+      <c r="C123" s="68"/>
+      <c r="D123" s="68"/>
       <c r="E123" s="23">
         <v>10</v>
       </c>
@@ -2683,12 +2683,12 @@
       </c>
     </row>
     <row r="124" spans="1:6">
-      <c r="A124" s="72" t="s">
+      <c r="A124" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="B124" s="72"/>
-      <c r="C124" s="72"/>
-      <c r="D124" s="72"/>
+      <c r="B124" s="68"/>
+      <c r="C124" s="68"/>
+      <c r="D124" s="68"/>
       <c r="E124" s="23">
         <v>50</v>
       </c>
@@ -2697,12 +2697,12 @@
       </c>
     </row>
     <row r="125" spans="1:6">
-      <c r="A125" s="73" t="s">
+      <c r="A125" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="B125" s="73"/>
-      <c r="C125" s="73"/>
-      <c r="D125" s="73"/>
+      <c r="B125" s="58"/>
+      <c r="C125" s="58"/>
+      <c r="D125" s="58"/>
       <c r="E125" s="23">
         <v>5</v>
       </c>
@@ -2711,12 +2711,12 @@
       </c>
     </row>
     <row r="126" spans="1:6">
-      <c r="A126" s="74" t="s">
+      <c r="A126" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="B126" s="74"/>
-      <c r="C126" s="74"/>
-      <c r="D126" s="74"/>
+      <c r="B126" s="67"/>
+      <c r="C126" s="67"/>
+      <c r="D126" s="67"/>
       <c r="E126" s="23">
         <v>10</v>
       </c>
@@ -2725,12 +2725,12 @@
       </c>
     </row>
     <row r="127" spans="1:6">
-      <c r="A127" s="74" t="s">
-        <v>10</v>
-      </c>
-      <c r="B127" s="74"/>
-      <c r="C127" s="74"/>
-      <c r="D127" s="74"/>
+      <c r="A127" s="67" t="s">
+        <v>10</v>
+      </c>
+      <c r="B127" s="67"/>
+      <c r="C127" s="67"/>
+      <c r="D127" s="67"/>
       <c r="E127" s="23">
         <v>15</v>
       </c>
@@ -2739,12 +2739,12 @@
       </c>
     </row>
     <row r="128" spans="1:6">
-      <c r="A128" s="73" t="s">
+      <c r="A128" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="B128" s="73"/>
-      <c r="C128" s="73"/>
-      <c r="D128" s="73"/>
+      <c r="B128" s="58"/>
+      <c r="C128" s="58"/>
+      <c r="D128" s="58"/>
       <c r="E128" s="13">
         <v>5</v>
       </c>
@@ -2753,12 +2753,12 @@
       </c>
     </row>
     <row r="129" spans="1:6">
-      <c r="A129" s="73" t="s">
+      <c r="A129" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="B129" s="73"/>
-      <c r="C129" s="73"/>
-      <c r="D129" s="73"/>
+      <c r="B129" s="58"/>
+      <c r="C129" s="58"/>
+      <c r="D129" s="58"/>
       <c r="E129" s="13">
         <v>7</v>
       </c>
@@ -2875,12 +2875,12 @@
       </c>
     </row>
     <row r="140" spans="1:6">
-      <c r="A140" s="77" t="s">
+      <c r="A140" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="B140" s="77"/>
-      <c r="C140" s="77"/>
-      <c r="D140" s="77"/>
+      <c r="B140" s="66"/>
+      <c r="C140" s="66"/>
+      <c r="D140" s="66"/>
       <c r="E140" s="13">
         <v>10</v>
       </c>
@@ -2889,12 +2889,12 @@
       </c>
     </row>
     <row r="141" spans="1:6">
-      <c r="A141" s="73" t="s">
+      <c r="A141" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="B141" s="73"/>
-      <c r="C141" s="73"/>
-      <c r="D141" s="73"/>
+      <c r="B141" s="58"/>
+      <c r="C141" s="58"/>
+      <c r="D141" s="58"/>
       <c r="E141" s="13">
         <v>30</v>
       </c>
@@ -2903,12 +2903,12 @@
       </c>
     </row>
     <row r="142" spans="1:6">
-      <c r="A142" s="73" t="s">
+      <c r="A142" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="B142" s="73"/>
-      <c r="C142" s="73"/>
-      <c r="D142" s="73"/>
+      <c r="B142" s="58"/>
+      <c r="C142" s="58"/>
+      <c r="D142" s="58"/>
       <c r="E142" s="13">
         <v>15</v>
       </c>
@@ -2917,12 +2917,12 @@
       </c>
     </row>
     <row r="143" spans="1:6">
-      <c r="A143" s="77" t="s">
+      <c r="A143" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="B143" s="77"/>
-      <c r="C143" s="77"/>
-      <c r="D143" s="77"/>
+      <c r="B143" s="66"/>
+      <c r="C143" s="66"/>
+      <c r="D143" s="66"/>
       <c r="E143" s="13">
         <v>50</v>
       </c>
@@ -2931,12 +2931,12 @@
       </c>
     </row>
     <row r="144" spans="1:6">
-      <c r="A144" s="77" t="s">
+      <c r="A144" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="B144" s="77"/>
-      <c r="C144" s="77"/>
-      <c r="D144" s="77"/>
+      <c r="B144" s="66"/>
+      <c r="C144" s="66"/>
+      <c r="D144" s="66"/>
       <c r="E144" s="13">
         <v>30</v>
       </c>
@@ -2945,12 +2945,12 @@
       </c>
     </row>
     <row r="145" spans="1:6">
-      <c r="A145" s="77" t="s">
+      <c r="A145" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="B145" s="77"/>
-      <c r="C145" s="77"/>
-      <c r="D145" s="77"/>
+      <c r="B145" s="66"/>
+      <c r="C145" s="66"/>
+      <c r="D145" s="66"/>
       <c r="E145" s="13">
         <v>50</v>
       </c>
@@ -2959,12 +2959,12 @@
       </c>
     </row>
     <row r="146" spans="1:6">
-      <c r="A146" s="73" t="s">
+      <c r="A146" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="B146" s="73"/>
-      <c r="C146" s="73"/>
-      <c r="D146" s="73"/>
+      <c r="B146" s="58"/>
+      <c r="C146" s="58"/>
+      <c r="D146" s="58"/>
       <c r="E146" s="13">
         <v>10</v>
       </c>
@@ -2973,12 +2973,12 @@
       </c>
     </row>
     <row r="147" spans="1:6">
-      <c r="A147" s="76" t="s">
+      <c r="A147" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="B147" s="76"/>
-      <c r="C147" s="76"/>
-      <c r="D147" s="76"/>
+      <c r="B147" s="59"/>
+      <c r="C147" s="59"/>
+      <c r="D147" s="59"/>
       <c r="E147" s="13">
         <v>10</v>
       </c>
@@ -2987,12 +2987,12 @@
       </c>
     </row>
     <row r="148" spans="1:6">
-      <c r="A148" s="76" t="s">
-        <v>10</v>
-      </c>
-      <c r="B148" s="76"/>
-      <c r="C148" s="76"/>
-      <c r="D148" s="76"/>
+      <c r="A148" s="59" t="s">
+        <v>10</v>
+      </c>
+      <c r="B148" s="59"/>
+      <c r="C148" s="59"/>
+      <c r="D148" s="59"/>
       <c r="E148" s="13">
         <v>15</v>
       </c>
@@ -3001,60 +3001,60 @@
       </c>
     </row>
     <row r="149" spans="1:6">
-      <c r="A149" s="76" t="s">
+      <c r="A149" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="B149" s="76"/>
-      <c r="C149" s="76"/>
-      <c r="D149" s="76"/>
+      <c r="B149" s="59"/>
+      <c r="C149" s="59"/>
+      <c r="D149" s="59"/>
       <c r="E149" s="4">
         <v>5</v>
       </c>
       <c r="F149" s="13"/>
     </row>
     <row r="150" spans="1:6">
-      <c r="A150" s="76" t="s">
+      <c r="A150" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="B150" s="76"/>
-      <c r="C150" s="76"/>
-      <c r="D150" s="76"/>
+      <c r="B150" s="59"/>
+      <c r="C150" s="59"/>
+      <c r="D150" s="59"/>
       <c r="E150" s="4">
         <v>10</v>
       </c>
       <c r="F150" s="13"/>
     </row>
     <row r="151" spans="1:6">
-      <c r="A151" s="76" t="s">
+      <c r="A151" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="B151" s="76"/>
-      <c r="C151" s="76"/>
-      <c r="D151" s="76"/>
+      <c r="B151" s="59"/>
+      <c r="C151" s="59"/>
+      <c r="D151" s="59"/>
       <c r="E151" s="4">
         <v>10</v>
       </c>
       <c r="F151" s="13"/>
     </row>
     <row r="152" spans="1:6">
-      <c r="A152" s="76" t="s">
+      <c r="A152" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="B152" s="76"/>
-      <c r="C152" s="76"/>
-      <c r="D152" s="76"/>
+      <c r="B152" s="59"/>
+      <c r="C152" s="59"/>
+      <c r="D152" s="59"/>
       <c r="E152" s="4">
         <v>15</v>
       </c>
       <c r="F152" s="13"/>
     </row>
     <row r="153" spans="1:6">
-      <c r="A153" s="73" t="s">
+      <c r="A153" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="B153" s="73"/>
-      <c r="C153" s="73"/>
-      <c r="D153" s="73"/>
+      <c r="B153" s="58"/>
+      <c r="C153" s="58"/>
+      <c r="D153" s="58"/>
       <c r="E153" s="4">
         <v>5</v>
       </c>
@@ -3063,12 +3063,12 @@
       </c>
     </row>
     <row r="154" spans="1:6">
-      <c r="A154" s="73" t="s">
+      <c r="A154" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="B154" s="73"/>
-      <c r="C154" s="73"/>
-      <c r="D154" s="73"/>
+      <c r="B154" s="58"/>
+      <c r="C154" s="58"/>
+      <c r="D154" s="58"/>
       <c r="E154" s="4">
         <v>7</v>
       </c>
@@ -3162,6 +3162,93 @@
     </row>
   </sheetData>
   <mergeCells count="111">
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="A50:D50"/>
+    <mergeCell ref="A51:D51"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="A52:D52"/>
+    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A56:D56"/>
+    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="A62:D62"/>
+    <mergeCell ref="A64:D64"/>
+    <mergeCell ref="A65:D65"/>
+    <mergeCell ref="A68:F68"/>
+    <mergeCell ref="A70:D70"/>
+    <mergeCell ref="A71:D71"/>
+    <mergeCell ref="A72:D72"/>
+    <mergeCell ref="A73:D73"/>
+    <mergeCell ref="A74:D74"/>
+    <mergeCell ref="A75:D75"/>
+    <mergeCell ref="A76:D76"/>
+    <mergeCell ref="A77:D77"/>
+    <mergeCell ref="A78:D78"/>
+    <mergeCell ref="A79:D79"/>
+    <mergeCell ref="A80:D80"/>
+    <mergeCell ref="A89:F89"/>
+    <mergeCell ref="A91:D91"/>
+    <mergeCell ref="A92:D92"/>
+    <mergeCell ref="A93:D93"/>
+    <mergeCell ref="A94:D94"/>
+    <mergeCell ref="A95:D95"/>
+    <mergeCell ref="A148:D148"/>
+    <mergeCell ref="A149:D149"/>
+    <mergeCell ref="A123:D123"/>
+    <mergeCell ref="A124:D124"/>
+    <mergeCell ref="A125:D125"/>
+    <mergeCell ref="A126:D126"/>
+    <mergeCell ref="A127:D127"/>
+    <mergeCell ref="A128:D128"/>
+    <mergeCell ref="A129:D129"/>
+    <mergeCell ref="A138:F138"/>
+    <mergeCell ref="A140:D140"/>
+    <mergeCell ref="A106:D106"/>
+    <mergeCell ref="A107:D107"/>
+    <mergeCell ref="A108:D108"/>
+    <mergeCell ref="A117:F117"/>
+    <mergeCell ref="A119:D119"/>
+    <mergeCell ref="A120:D120"/>
+    <mergeCell ref="A121:D121"/>
+    <mergeCell ref="A122:D122"/>
+    <mergeCell ref="A96:D96"/>
+    <mergeCell ref="A97:D97"/>
+    <mergeCell ref="A98:D98"/>
+    <mergeCell ref="A99:D99"/>
+    <mergeCell ref="A100:D100"/>
+    <mergeCell ref="A101:D101"/>
+    <mergeCell ref="A102:D102"/>
+    <mergeCell ref="A103:D103"/>
+    <mergeCell ref="A104:D104"/>
     <mergeCell ref="J22:M22"/>
     <mergeCell ref="A150:D150"/>
     <mergeCell ref="A151:D151"/>
@@ -3186,93 +3273,6 @@
     <mergeCell ref="A146:D146"/>
     <mergeCell ref="A147:D147"/>
     <mergeCell ref="A105:D105"/>
-    <mergeCell ref="A106:D106"/>
-    <mergeCell ref="A107:D107"/>
-    <mergeCell ref="A108:D108"/>
-    <mergeCell ref="A117:F117"/>
-    <mergeCell ref="A119:D119"/>
-    <mergeCell ref="A120:D120"/>
-    <mergeCell ref="A121:D121"/>
-    <mergeCell ref="A122:D122"/>
-    <mergeCell ref="A96:D96"/>
-    <mergeCell ref="A97:D97"/>
-    <mergeCell ref="A98:D98"/>
-    <mergeCell ref="A99:D99"/>
-    <mergeCell ref="A100:D100"/>
-    <mergeCell ref="A101:D101"/>
-    <mergeCell ref="A148:D148"/>
-    <mergeCell ref="A149:D149"/>
-    <mergeCell ref="A123:D123"/>
-    <mergeCell ref="A124:D124"/>
-    <mergeCell ref="A125:D125"/>
-    <mergeCell ref="A126:D126"/>
-    <mergeCell ref="A127:D127"/>
-    <mergeCell ref="A128:D128"/>
-    <mergeCell ref="A129:D129"/>
-    <mergeCell ref="A138:F138"/>
-    <mergeCell ref="A140:D140"/>
-    <mergeCell ref="A102:D102"/>
-    <mergeCell ref="A103:D103"/>
-    <mergeCell ref="A104:D104"/>
-    <mergeCell ref="A78:D78"/>
-    <mergeCell ref="A79:D79"/>
-    <mergeCell ref="A80:D80"/>
-    <mergeCell ref="A89:F89"/>
-    <mergeCell ref="A91:D91"/>
-    <mergeCell ref="A92:D92"/>
-    <mergeCell ref="A93:D93"/>
-    <mergeCell ref="A94:D94"/>
-    <mergeCell ref="A95:D95"/>
-    <mergeCell ref="A68:F68"/>
-    <mergeCell ref="A70:D70"/>
-    <mergeCell ref="A71:D71"/>
-    <mergeCell ref="A72:D72"/>
-    <mergeCell ref="A73:D73"/>
-    <mergeCell ref="A74:D74"/>
-    <mergeCell ref="A75:D75"/>
-    <mergeCell ref="A76:D76"/>
-    <mergeCell ref="A77:D77"/>
-    <mergeCell ref="A53:D53"/>
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A56:D56"/>
-    <mergeCell ref="A57:D57"/>
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="A62:D62"/>
-    <mergeCell ref="A64:D64"/>
-    <mergeCell ref="A65:D65"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="A49:D49"/>
-    <mergeCell ref="A50:D50"/>
-    <mergeCell ref="A51:D51"/>
-    <mergeCell ref="F51:F52"/>
-    <mergeCell ref="A52:D52"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A22:F22"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:D11"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
preparação para futuras modificações
</commit_message>
<xml_diff>
--- a/Planilha geral.xlsx
+++ b/Planilha geral.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="77">
   <si>
     <t>EXATAS</t>
   </si>
@@ -203,6 +203,54 @@
   </si>
   <si>
     <t>Requisitos que faltam ser implementados</t>
+  </si>
+  <si>
+    <t>setOrientacaoDoutoradoConcluida</t>
+  </si>
+  <si>
+    <t>setOrientacaoMestradoConcluida</t>
+  </si>
+  <si>
+    <t>setOrientacaoEmAndamento</t>
+  </si>
+  <si>
+    <t>Antes</t>
+  </si>
+  <si>
+    <t>setOrientacaoEmAndamento + setOrientacaoDoutoradoConcluida</t>
+  </si>
+  <si>
+    <t>setOrientacaoEmAndamento + setOrientacaoMestradoConcluida</t>
+  </si>
+  <si>
+    <t>Depois</t>
+  </si>
+  <si>
+    <t>setOrientacaoDouAndConclu</t>
+  </si>
+  <si>
+    <t>setCorientacaoDouAndConclu</t>
+  </si>
+  <si>
+    <t>setOrientacaoMesAndConclu</t>
+  </si>
+  <si>
+    <t>setCorientacaoMesAndConclu</t>
+  </si>
+  <si>
+    <t>setCorientacaoDoutoradoConcluida</t>
+  </si>
+  <si>
+    <t>setCorientacaoMestradoConcluida</t>
+  </si>
+  <si>
+    <t>Situação</t>
+  </si>
+  <si>
+    <t>Orientação TFC</t>
+  </si>
+  <si>
+    <t>Ver email do Ciro</t>
   </si>
 </sst>
 </file>
@@ -263,7 +311,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -438,12 +486,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -522,45 +610,62 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -924,10 +1029,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:O160"/>
+  <dimension ref="A2:U160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A86" sqref="A86"/>
+    <sheetView tabSelected="1" topLeftCell="G31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O48" sqref="O48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -939,18 +1044,22 @@
     <col min="7" max="7" width="14.28515625" customWidth="1"/>
     <col min="8" max="12" width="8.85546875"/>
     <col min="13" max="13" width="29" customWidth="1"/>
-    <col min="14" max="1025" width="8.85546875"/>
+    <col min="14" max="14" width="14.85546875" customWidth="1"/>
+    <col min="15" max="15" width="47.85546875" customWidth="1"/>
+    <col min="16" max="17" width="8.85546875"/>
+    <col min="18" max="18" width="10.42578125" customWidth="1"/>
+    <col min="19" max="1025" width="8.85546875"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:15" ht="14.25" customHeight="1">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
     </row>
     <row r="3" spans="1:15" ht="14.25" customHeight="1">
       <c r="A3" s="39" t="s">
@@ -967,12 +1076,12 @@
       </c>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="77"/>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
       <c r="E4" s="48">
         <v>10</v>
       </c>
@@ -984,216 +1093,216 @@
       </c>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="78" t="s">
+      <c r="A5" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="78"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
       <c r="E5" s="48">
         <v>15</v>
       </c>
       <c r="F5" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="61" t="s">
+      <c r="J5" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="K5" s="61"/>
-      <c r="L5" s="61"/>
-      <c r="M5" s="61"/>
+      <c r="K5" s="66"/>
+      <c r="L5" s="66"/>
+      <c r="M5" s="66"/>
       <c r="N5" s="12" t="s">
         <v>25</v>
       </c>
       <c r="O5" s="23"/>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="78" t="s">
+      <c r="A6" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="78"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
+      <c r="B6" s="64"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
       <c r="E6" s="48">
         <v>8</v>
       </c>
       <c r="F6" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="J6" s="62" t="s">
+      <c r="J6" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="K6" s="62"/>
-      <c r="L6" s="62"/>
-      <c r="M6" s="62"/>
+      <c r="K6" s="67"/>
+      <c r="L6" s="67"/>
+      <c r="M6" s="67"/>
       <c r="N6" s="14" t="s">
         <v>27</v>
       </c>
       <c r="O6" s="23"/>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" s="77" t="s">
+      <c r="A7" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="77"/>
-      <c r="C7" s="77"/>
-      <c r="D7" s="77"/>
+      <c r="B7" s="63"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="63"/>
       <c r="E7" s="48">
         <v>20</v>
       </c>
       <c r="F7" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="J7" s="63" t="s">
+      <c r="J7" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="63"/>
-      <c r="L7" s="63"/>
-      <c r="M7" s="63"/>
+      <c r="K7" s="80"/>
+      <c r="L7" s="80"/>
+      <c r="M7" s="80"/>
       <c r="N7" s="4">
         <v>5</v>
       </c>
       <c r="O7" s="2"/>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="77" t="s">
+      <c r="A8" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="77"/>
-      <c r="C8" s="77"/>
-      <c r="D8" s="77"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
       <c r="E8" s="48">
         <v>10</v>
       </c>
       <c r="F8" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="J8" s="63" t="s">
+      <c r="J8" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="63"/>
-      <c r="L8" s="63"/>
-      <c r="M8" s="63"/>
+      <c r="K8" s="80"/>
+      <c r="L8" s="80"/>
+      <c r="M8" s="80"/>
       <c r="N8" s="4">
         <v>10</v>
       </c>
       <c r="O8" s="2"/>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="77" t="s">
+      <c r="A9" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="77"/>
-      <c r="C9" s="77"/>
-      <c r="D9" s="77"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="63"/>
       <c r="E9" s="48">
         <v>5</v>
       </c>
       <c r="F9" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="J9" s="63" t="s">
+      <c r="J9" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="63"/>
-      <c r="L9" s="63"/>
-      <c r="M9" s="63"/>
+      <c r="K9" s="80"/>
+      <c r="L9" s="80"/>
+      <c r="M9" s="80"/>
       <c r="N9" s="4">
         <v>10</v>
       </c>
       <c r="O9" s="2"/>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10" s="78" t="s">
+      <c r="A10" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="78"/>
-      <c r="C10" s="78"/>
-      <c r="D10" s="78"/>
+      <c r="B10" s="64"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="64"/>
       <c r="E10" s="48">
         <v>3</v>
       </c>
       <c r="F10" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="J10" s="63" t="s">
+      <c r="J10" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="K10" s="63"/>
-      <c r="L10" s="63"/>
-      <c r="M10" s="63"/>
+      <c r="K10" s="80"/>
+      <c r="L10" s="80"/>
+      <c r="M10" s="80"/>
       <c r="N10" s="4">
         <v>15</v>
       </c>
       <c r="O10" s="2"/>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11" s="75" t="s">
+      <c r="A11" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="75"/>
-      <c r="C11" s="75"/>
-      <c r="D11" s="75"/>
+      <c r="B11" s="60"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
       <c r="E11" s="48">
         <v>10</v>
       </c>
       <c r="F11" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="J11" s="64" t="s">
+      <c r="J11" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="K11" s="64"/>
-      <c r="L11" s="64"/>
-      <c r="M11" s="64"/>
+      <c r="K11" s="70"/>
+      <c r="L11" s="70"/>
+      <c r="M11" s="70"/>
     </row>
     <row r="12" spans="1:15">
-      <c r="A12" s="75" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="75"/>
-      <c r="C12" s="75"/>
-      <c r="D12" s="75"/>
+      <c r="A12" s="60" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="60"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="60"/>
       <c r="E12" s="48">
         <v>15</v>
       </c>
       <c r="F12" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="J12" s="64" t="s">
+      <c r="J12" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="K12" s="64"/>
-      <c r="L12" s="64"/>
-      <c r="M12" s="64"/>
+      <c r="K12" s="70"/>
+      <c r="L12" s="70"/>
+      <c r="M12" s="70"/>
     </row>
     <row r="13" spans="1:15">
-      <c r="A13" s="76" t="s">
+      <c r="A13" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="76"/>
-      <c r="C13" s="76"/>
-      <c r="D13" s="76"/>
+      <c r="B13" s="61"/>
+      <c r="C13" s="61"/>
+      <c r="D13" s="61"/>
       <c r="E13" s="49">
         <v>5</v>
       </c>
       <c r="F13" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="J13" s="65" t="s">
+      <c r="J13" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="65"/>
-      <c r="L13" s="65"/>
-      <c r="M13" s="65"/>
+      <c r="K13" s="71"/>
+      <c r="L13" s="71"/>
+      <c r="M13" s="71"/>
     </row>
     <row r="14" spans="1:15">
-      <c r="A14" s="76" t="s">
+      <c r="A14" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="76"/>
-      <c r="C14" s="76"/>
-      <c r="D14" s="76"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="61"/>
       <c r="E14" s="49">
         <v>7</v>
       </c>
@@ -1247,7 +1356,7 @@
       <c r="L16" s="56"/>
       <c r="M16" s="56"/>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:21">
       <c r="A17" s="50" t="s">
         <v>19</v>
       </c>
@@ -1267,7 +1376,7 @@
       <c r="L17" s="55"/>
       <c r="M17" s="55"/>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:21">
       <c r="A18" s="50" t="s">
         <v>20</v>
       </c>
@@ -1287,7 +1396,7 @@
       <c r="L18" s="55"/>
       <c r="M18" s="55"/>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:21">
       <c r="A19" s="50" t="s">
         <v>21</v>
       </c>
@@ -1307,7 +1416,7 @@
       <c r="L19" s="56"/>
       <c r="M19" s="56"/>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:21">
       <c r="A20" s="53" t="s">
         <v>22</v>
       </c>
@@ -1327,7 +1436,7 @@
       <c r="L20" s="56"/>
       <c r="M20" s="56"/>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:21">
       <c r="A21" s="40"/>
       <c r="B21" s="41"/>
       <c r="C21" s="41"/>
@@ -1341,23 +1450,23 @@
       <c r="L21" s="55"/>
       <c r="M21" s="55"/>
     </row>
-    <row r="22" spans="1:13">
-      <c r="A22" s="60" t="s">
+    <row r="22" spans="1:21">
+      <c r="A22" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="60"/>
-      <c r="C22" s="60"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="60"/>
-      <c r="F22" s="60"/>
-      <c r="J22" s="58" t="s">
+      <c r="B22" s="62"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="62"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="62"/>
+      <c r="J22" s="75" t="s">
         <v>53</v>
       </c>
-      <c r="K22" s="58"/>
-      <c r="L22" s="58"/>
-      <c r="M22" s="58"/>
-    </row>
-    <row r="23" spans="1:13">
+      <c r="K22" s="75"/>
+      <c r="L22" s="75"/>
+      <c r="M22" s="75"/>
+    </row>
+    <row r="23" spans="1:21">
       <c r="A23" s="39" t="s">
         <v>56</v>
       </c>
@@ -1371,13 +1480,13 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
-      <c r="A24" s="72" t="s">
+    <row r="24" spans="1:21">
+      <c r="A24" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="72"/>
-      <c r="C24" s="72"/>
-      <c r="D24" s="72"/>
+      <c r="B24" s="65"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="65"/>
       <c r="E24" s="10">
         <v>10</v>
       </c>
@@ -1385,116 +1494,205 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
-      <c r="A25" s="61" t="s">
+    <row r="25" spans="1:21">
+      <c r="A25" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="61"/>
-      <c r="C25" s="61"/>
-      <c r="D25" s="61"/>
+      <c r="B25" s="66"/>
+      <c r="C25" s="66"/>
+      <c r="D25" s="66"/>
       <c r="E25" s="12" t="s">
         <v>25</v>
       </c>
       <c r="F25" s="13"/>
     </row>
-    <row r="26" spans="1:13">
-      <c r="A26" s="62" t="s">
+    <row r="26" spans="1:21">
+      <c r="A26" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="62"/>
-      <c r="C26" s="62"/>
-      <c r="D26" s="62"/>
+      <c r="B26" s="67"/>
+      <c r="C26" s="67"/>
+      <c r="D26" s="67"/>
       <c r="E26" s="14" t="s">
         <v>27</v>
       </c>
       <c r="F26" s="13"/>
     </row>
-    <row r="27" spans="1:13">
-      <c r="A27" s="72" t="s">
+    <row r="27" spans="1:21">
+      <c r="A27" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="72"/>
-      <c r="C27" s="72"/>
-      <c r="D27" s="72"/>
+      <c r="B27" s="65"/>
+      <c r="C27" s="65"/>
+      <c r="D27" s="65"/>
       <c r="E27" s="10">
         <v>15</v>
       </c>
       <c r="F27" s="13" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:13">
-      <c r="A28" s="72" t="s">
+      <c r="N27" s="81" t="s">
+        <v>64</v>
+      </c>
+      <c r="O27" s="81"/>
+      <c r="P27" t="s">
+        <v>67</v>
+      </c>
+      <c r="T27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21">
+      <c r="A28" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="72"/>
-      <c r="C28" s="72"/>
-      <c r="D28" s="72"/>
+      <c r="B28" s="65"/>
+      <c r="C28" s="65"/>
+      <c r="D28" s="65"/>
       <c r="E28" s="10">
         <v>10</v>
       </c>
       <c r="F28" s="13" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:13">
-      <c r="A29" s="73" t="s">
+      <c r="J28" s="51" t="s">
+        <v>18</v>
+      </c>
+      <c r="K28" s="91"/>
+      <c r="L28" s="91"/>
+      <c r="M28" s="91"/>
+      <c r="N28" s="85" t="s">
+        <v>65</v>
+      </c>
+      <c r="O28" s="85"/>
+      <c r="P28" s="85" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q28" s="85"/>
+      <c r="R28" s="85"/>
+      <c r="S28" s="85"/>
+      <c r="T28" s="88"/>
+      <c r="U28" s="41"/>
+    </row>
+    <row r="29" spans="1:21">
+      <c r="A29" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="73"/>
-      <c r="C29" s="73"/>
-      <c r="D29" s="73"/>
+      <c r="B29" s="68"/>
+      <c r="C29" s="68"/>
+      <c r="D29" s="68"/>
       <c r="E29" s="10">
         <v>10</v>
       </c>
       <c r="F29" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="M29" s="57"/>
-    </row>
-    <row r="30" spans="1:13">
-      <c r="A30" s="73" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" s="73"/>
-      <c r="C30" s="73"/>
-      <c r="D30" s="73"/>
+      <c r="J29" s="51" t="s">
+        <v>19</v>
+      </c>
+      <c r="K29" s="91"/>
+      <c r="L29" s="91"/>
+      <c r="M29" s="92"/>
+      <c r="N29" s="86" t="s">
+        <v>65</v>
+      </c>
+      <c r="O29" s="86"/>
+      <c r="P29" s="85" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q29" s="85"/>
+      <c r="R29" s="85"/>
+      <c r="S29" s="85"/>
+      <c r="T29" s="88"/>
+      <c r="U29" s="41"/>
+    </row>
+    <row r="30" spans="1:21">
+      <c r="A30" s="68" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="68"/>
+      <c r="C30" s="68"/>
+      <c r="D30" s="68"/>
       <c r="E30" s="10">
         <v>15</v>
       </c>
       <c r="F30" s="13" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:13">
-      <c r="A31" s="74" t="s">
+      <c r="J30" s="51" t="s">
+        <v>20</v>
+      </c>
+      <c r="K30" s="91"/>
+      <c r="L30" s="91"/>
+      <c r="M30" s="91"/>
+      <c r="N30" s="86" t="s">
+        <v>66</v>
+      </c>
+      <c r="O30" s="86"/>
+      <c r="P30" s="85" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q30" s="85"/>
+      <c r="R30" s="85"/>
+      <c r="S30" s="85"/>
+      <c r="T30" s="88"/>
+      <c r="U30" s="82"/>
+    </row>
+    <row r="31" spans="1:21">
+      <c r="A31" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="74"/>
-      <c r="C31" s="74"/>
-      <c r="D31" s="74"/>
+      <c r="B31" s="69"/>
+      <c r="C31" s="69"/>
+      <c r="D31" s="69"/>
       <c r="E31" s="11">
         <v>5</v>
       </c>
       <c r="F31" s="13" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:13">
-      <c r="A32" s="74" t="s">
+      <c r="J31" s="51" t="s">
+        <v>21</v>
+      </c>
+      <c r="K31" s="91"/>
+      <c r="L31" s="91"/>
+      <c r="M31" s="91"/>
+      <c r="N31" s="86" t="s">
+        <v>66</v>
+      </c>
+      <c r="O31" s="86"/>
+      <c r="P31" s="85" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q31" s="85"/>
+      <c r="R31" s="85"/>
+      <c r="S31" s="85"/>
+      <c r="T31" s="88"/>
+      <c r="U31" s="82"/>
+    </row>
+    <row r="32" spans="1:21">
+      <c r="A32" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="74"/>
-      <c r="C32" s="74"/>
-      <c r="D32" s="74"/>
+      <c r="B32" s="69"/>
+      <c r="C32" s="69"/>
+      <c r="D32" s="69"/>
       <c r="E32" s="11">
         <v>7</v>
       </c>
       <c r="F32" s="13" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:7">
+      <c r="J32" s="40"/>
+      <c r="N32" s="81"/>
+      <c r="O32" s="81"/>
+      <c r="P32" s="81"/>
+      <c r="Q32" s="81"/>
+      <c r="R32" s="81"/>
+      <c r="S32" s="89"/>
+      <c r="T32" s="83"/>
+    </row>
+    <row r="33" spans="1:21">
       <c r="A33" s="15" t="s">
         <v>17</v>
       </c>
@@ -1507,8 +1705,15 @@
       <c r="F33" s="13" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:7">
+      <c r="N33" s="81"/>
+      <c r="O33" s="81"/>
+      <c r="P33" s="84"/>
+      <c r="Q33" s="84"/>
+      <c r="R33" s="84"/>
+      <c r="S33" s="90"/>
+      <c r="T33" s="83"/>
+    </row>
+    <row r="34" spans="1:21">
       <c r="A34" s="15" t="s">
         <v>18</v>
       </c>
@@ -1521,8 +1726,26 @@
       <c r="F34" s="13" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:7">
+      <c r="J34" s="58" t="s">
+        <v>36</v>
+      </c>
+      <c r="K34" s="58"/>
+      <c r="L34" s="58"/>
+      <c r="M34" s="59"/>
+      <c r="N34" s="86" t="s">
+        <v>63</v>
+      </c>
+      <c r="O34" s="87"/>
+      <c r="P34" s="85" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q34" s="85"/>
+      <c r="R34" s="85"/>
+      <c r="S34" s="85"/>
+      <c r="T34" s="88"/>
+      <c r="U34" s="41"/>
+    </row>
+    <row r="35" spans="1:21">
       <c r="A35" s="17" t="s">
         <v>19</v>
       </c>
@@ -1535,8 +1758,26 @@
       <c r="F35" s="13" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:7">
+      <c r="J35" s="58" t="s">
+        <v>37</v>
+      </c>
+      <c r="K35" s="58"/>
+      <c r="L35" s="58"/>
+      <c r="M35" s="59"/>
+      <c r="N35" s="86" t="s">
+        <v>63</v>
+      </c>
+      <c r="O35" s="87"/>
+      <c r="P35" s="85" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q35" s="85"/>
+      <c r="R35" s="85"/>
+      <c r="S35" s="85"/>
+      <c r="T35" s="88"/>
+      <c r="U35" s="41"/>
+    </row>
+    <row r="36" spans="1:21">
       <c r="A36" s="17" t="s">
         <v>20</v>
       </c>
@@ -1549,8 +1790,26 @@
       <c r="F36" s="13" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:7">
+      <c r="J36" s="70" t="s">
+        <v>38</v>
+      </c>
+      <c r="K36" s="70"/>
+      <c r="L36" s="70"/>
+      <c r="M36" s="73"/>
+      <c r="N36" s="86" t="s">
+        <v>61</v>
+      </c>
+      <c r="O36" s="87"/>
+      <c r="P36" s="85" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q36" s="85"/>
+      <c r="R36" s="85"/>
+      <c r="S36" s="85"/>
+      <c r="T36" s="88"/>
+      <c r="U36" s="41"/>
+    </row>
+    <row r="37" spans="1:21">
       <c r="A37" s="17" t="s">
         <v>21</v>
       </c>
@@ -1563,8 +1822,26 @@
       <c r="F37" s="13" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:7">
+      <c r="J37" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="K37" s="59"/>
+      <c r="L37" s="59"/>
+      <c r="M37" s="59"/>
+      <c r="N37" s="86" t="s">
+        <v>62</v>
+      </c>
+      <c r="O37" s="87"/>
+      <c r="P37" s="85" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q37" s="85"/>
+      <c r="R37" s="85"/>
+      <c r="S37" s="85"/>
+      <c r="T37" s="88"/>
+      <c r="U37" s="82"/>
+    </row>
+    <row r="38" spans="1:21">
       <c r="A38" s="20" t="s">
         <v>22</v>
       </c>
@@ -1577,22 +1854,63 @@
       <c r="F38" s="23" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:7">
+      <c r="J38" s="73" t="s">
+        <v>40</v>
+      </c>
+      <c r="K38" s="73"/>
+      <c r="L38" s="73"/>
+      <c r="M38" s="73"/>
+      <c r="N38" s="86" t="s">
+        <v>61</v>
+      </c>
+      <c r="O38" s="87"/>
+      <c r="P38" s="85" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q38" s="85"/>
+      <c r="R38" s="85"/>
+      <c r="S38" s="85"/>
+      <c r="T38" s="88"/>
+      <c r="U38" s="41"/>
+    </row>
+    <row r="39" spans="1:21">
+      <c r="J39" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="K39" s="59"/>
+      <c r="L39" s="59"/>
+      <c r="M39" s="59"/>
+      <c r="N39" s="86" t="s">
+        <v>62</v>
+      </c>
+      <c r="O39" s="87"/>
+      <c r="P39" s="85" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q39" s="85"/>
+      <c r="R39" s="85"/>
+      <c r="S39" s="85"/>
+      <c r="T39" s="88"/>
+      <c r="U39" s="82"/>
+    </row>
+    <row r="40" spans="1:21">
       <c r="G40" s="1"/>
     </row>
-    <row r="41" spans="1:7">
-      <c r="A41" s="60" t="s">
+    <row r="41" spans="1:21">
+      <c r="A41" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="B41" s="60"/>
-      <c r="C41" s="60"/>
-      <c r="D41" s="60"/>
-      <c r="E41" s="60"/>
-      <c r="F41" s="60"/>
-      <c r="G41" s="60"/>
-    </row>
-    <row r="42" spans="1:7">
+      <c r="B41" s="62"/>
+      <c r="C41" s="62"/>
+      <c r="D41" s="62"/>
+      <c r="E41" s="62"/>
+      <c r="F41" s="62"/>
+      <c r="G41" s="62"/>
+      <c r="J41" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21">
       <c r="A42" s="39" t="s">
         <v>56</v>
       </c>
@@ -1609,13 +1927,13 @@
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
-      <c r="A43" s="64" t="s">
+    <row r="43" spans="1:21">
+      <c r="A43" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="B43" s="64"/>
-      <c r="C43" s="64"/>
-      <c r="D43" s="64"/>
+      <c r="B43" s="70"/>
+      <c r="C43" s="70"/>
+      <c r="D43" s="70"/>
       <c r="E43" s="25">
         <v>10</v>
       </c>
@@ -1625,14 +1943,21 @@
       <c r="G43" s="26" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:7">
-      <c r="A44" s="64" t="s">
+      <c r="J43" s="93" t="s">
+        <v>76</v>
+      </c>
+      <c r="K43" s="93"/>
+      <c r="L43" s="93"/>
+      <c r="M43" s="93"/>
+      <c r="N43" s="93"/>
+    </row>
+    <row r="44" spans="1:21">
+      <c r="A44" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="B44" s="64"/>
-      <c r="C44" s="64"/>
-      <c r="D44" s="64"/>
+      <c r="B44" s="70"/>
+      <c r="C44" s="70"/>
+      <c r="D44" s="70"/>
       <c r="E44" s="25">
         <v>16</v>
       </c>
@@ -1640,14 +1965,19 @@
         <v>29</v>
       </c>
       <c r="G44" s="26"/>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="A45" s="64" t="s">
+      <c r="J44" s="93"/>
+      <c r="K44" s="93"/>
+      <c r="L44" s="93"/>
+      <c r="M44" s="93"/>
+      <c r="N44" s="93"/>
+    </row>
+    <row r="45" spans="1:21">
+      <c r="A45" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="B45" s="64"/>
-      <c r="C45" s="64"/>
-      <c r="D45" s="64"/>
+      <c r="B45" s="70"/>
+      <c r="C45" s="70"/>
+      <c r="D45" s="70"/>
       <c r="E45" s="25">
         <v>10</v>
       </c>
@@ -1656,13 +1986,13 @@
       </c>
       <c r="G45" s="26"/>
     </row>
-    <row r="46" spans="1:7">
-      <c r="A46" s="65" t="s">
+    <row r="46" spans="1:21">
+      <c r="A46" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="B46" s="65"/>
-      <c r="C46" s="65"/>
-      <c r="D46" s="65"/>
+      <c r="B46" s="71"/>
+      <c r="C46" s="71"/>
+      <c r="D46" s="71"/>
       <c r="E46" s="25">
         <v>8</v>
       </c>
@@ -1671,7 +2001,7 @@
       </c>
       <c r="G46" s="26"/>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:21">
       <c r="A47" s="27" t="s">
         <v>33</v>
       </c>
@@ -1686,13 +2016,13 @@
       </c>
       <c r="G47" s="26"/>
     </row>
-    <row r="48" spans="1:7">
-      <c r="A48" s="64" t="s">
+    <row r="48" spans="1:21">
+      <c r="A48" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="B48" s="64"/>
-      <c r="C48" s="64"/>
-      <c r="D48" s="64"/>
+      <c r="B48" s="70"/>
+      <c r="C48" s="70"/>
+      <c r="D48" s="70"/>
       <c r="E48" s="25">
         <v>15</v>
       </c>
@@ -1702,14 +2032,15 @@
       <c r="G48" s="26" t="s">
         <v>2</v>
       </c>
+      <c r="O48" s="57"/>
     </row>
     <row r="49" spans="1:7">
-      <c r="A49" s="64" t="s">
+      <c r="A49" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="B49" s="64"/>
-      <c r="C49" s="64"/>
-      <c r="D49" s="64"/>
+      <c r="B49" s="70"/>
+      <c r="C49" s="70"/>
+      <c r="D49" s="70"/>
       <c r="E49" s="25">
         <v>5</v>
       </c>
@@ -1721,12 +2052,12 @@
       </c>
     </row>
     <row r="50" spans="1:7">
-      <c r="A50" s="64" t="s">
+      <c r="A50" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="B50" s="64"/>
-      <c r="C50" s="64"/>
-      <c r="D50" s="64"/>
+      <c r="B50" s="70"/>
+      <c r="C50" s="70"/>
+      <c r="D50" s="70"/>
       <c r="E50" s="25">
         <v>0</v>
       </c>
@@ -1738,40 +2069,40 @@
       </c>
     </row>
     <row r="51" spans="1:7">
-      <c r="A51" s="65" t="s">
+      <c r="A51" s="71" t="s">
         <v>34</v>
       </c>
-      <c r="B51" s="65"/>
-      <c r="C51" s="65"/>
-      <c r="D51" s="65"/>
+      <c r="B51" s="71"/>
+      <c r="C51" s="71"/>
+      <c r="D51" s="71"/>
       <c r="E51" s="25">
         <v>6</v>
       </c>
-      <c r="F51" s="71">
+      <c r="F51" s="72">
         <v>9</v>
       </c>
       <c r="G51" s="26"/>
     </row>
     <row r="52" spans="1:7">
-      <c r="A52" s="64" t="s">
+      <c r="A52" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="B52" s="64"/>
-      <c r="C52" s="64"/>
-      <c r="D52" s="64"/>
+      <c r="B52" s="70"/>
+      <c r="C52" s="70"/>
+      <c r="D52" s="70"/>
       <c r="E52" s="25">
         <v>4</v>
       </c>
-      <c r="F52" s="71"/>
+      <c r="F52" s="72"/>
       <c r="G52" s="26"/>
     </row>
     <row r="53" spans="1:7">
-      <c r="A53" s="65" t="s">
+      <c r="A53" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="B53" s="65"/>
-      <c r="C53" s="65"/>
-      <c r="D53" s="65"/>
+      <c r="B53" s="71"/>
+      <c r="C53" s="71"/>
+      <c r="D53" s="71"/>
       <c r="E53" s="25">
         <v>10</v>
       </c>
@@ -1783,12 +2114,12 @@
       </c>
     </row>
     <row r="54" spans="1:7">
-      <c r="A54" s="65" t="s">
-        <v>10</v>
-      </c>
-      <c r="B54" s="65"/>
-      <c r="C54" s="65"/>
-      <c r="D54" s="65"/>
+      <c r="A54" s="71" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" s="71"/>
+      <c r="C54" s="71"/>
+      <c r="D54" s="71"/>
       <c r="E54" s="25">
         <v>15</v>
       </c>
@@ -1800,12 +2131,12 @@
       </c>
     </row>
     <row r="55" spans="1:7">
-      <c r="A55" s="64" t="s">
+      <c r="A55" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="B55" s="64"/>
-      <c r="C55" s="64"/>
-      <c r="D55" s="64"/>
+      <c r="B55" s="70"/>
+      <c r="C55" s="70"/>
+      <c r="D55" s="70"/>
       <c r="E55" s="25">
         <v>1</v>
       </c>
@@ -1817,12 +2148,12 @@
       </c>
     </row>
     <row r="56" spans="1:7">
-      <c r="A56" s="64" t="s">
+      <c r="A56" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="B56" s="64"/>
-      <c r="C56" s="64"/>
-      <c r="D56" s="64"/>
+      <c r="B56" s="70"/>
+      <c r="C56" s="70"/>
+      <c r="D56" s="70"/>
       <c r="E56" s="25">
         <v>2</v>
       </c>
@@ -1834,12 +2165,12 @@
       </c>
     </row>
     <row r="57" spans="1:7">
-      <c r="A57" s="64" t="s">
+      <c r="A57" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="B57" s="64"/>
-      <c r="C57" s="64"/>
-      <c r="D57" s="64"/>
+      <c r="B57" s="70"/>
+      <c r="C57" s="70"/>
+      <c r="D57" s="70"/>
       <c r="E57" s="25">
         <v>1.5</v>
       </c>
@@ -1885,12 +2216,12 @@
       </c>
     </row>
     <row r="60" spans="1:7">
-      <c r="A60" s="64" t="s">
+      <c r="A60" s="70" t="s">
         <v>38</v>
       </c>
-      <c r="B60" s="64"/>
-      <c r="C60" s="64"/>
-      <c r="D60" s="64"/>
+      <c r="B60" s="70"/>
+      <c r="C60" s="70"/>
+      <c r="D60" s="70"/>
       <c r="E60" s="25">
         <v>10</v>
       </c>
@@ -1919,12 +2250,12 @@
       </c>
     </row>
     <row r="62" spans="1:7">
-      <c r="A62" s="70" t="s">
+      <c r="A62" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="B62" s="70"/>
-      <c r="C62" s="70"/>
-      <c r="D62" s="70"/>
+      <c r="B62" s="73"/>
+      <c r="C62" s="73"/>
+      <c r="D62" s="73"/>
       <c r="E62" s="25">
         <v>2</v>
       </c>
@@ -1953,12 +2284,12 @@
       </c>
     </row>
     <row r="64" spans="1:7">
-      <c r="A64" s="70" t="s">
+      <c r="A64" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="B64" s="70"/>
-      <c r="C64" s="70"/>
-      <c r="D64" s="70"/>
+      <c r="B64" s="73"/>
+      <c r="C64" s="73"/>
+      <c r="D64" s="73"/>
       <c r="E64" s="25">
         <v>0.5</v>
       </c>
@@ -1968,12 +2299,12 @@
       <c r="G64" s="26"/>
     </row>
     <row r="65" spans="1:7">
-      <c r="A65" s="70" t="s">
+      <c r="A65" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="B65" s="70"/>
-      <c r="C65" s="70"/>
-      <c r="D65" s="70"/>
+      <c r="B65" s="73"/>
+      <c r="C65" s="73"/>
+      <c r="D65" s="73"/>
       <c r="E65" s="25">
         <v>3</v>
       </c>
@@ -1985,14 +2316,14 @@
       </c>
     </row>
     <row r="68" spans="1:7">
-      <c r="A68" s="60" t="s">
+      <c r="A68" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="B68" s="60"/>
-      <c r="C68" s="60"/>
-      <c r="D68" s="60"/>
-      <c r="E68" s="60"/>
-      <c r="F68" s="60"/>
+      <c r="B68" s="62"/>
+      <c r="C68" s="62"/>
+      <c r="D68" s="62"/>
+      <c r="E68" s="62"/>
+      <c r="F68" s="62"/>
     </row>
     <row r="69" spans="1:7">
       <c r="A69" s="39" t="s">
@@ -2009,12 +2340,12 @@
       </c>
     </row>
     <row r="70" spans="1:7">
-      <c r="A70" s="68" t="s">
+      <c r="A70" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="B70" s="68"/>
-      <c r="C70" s="68"/>
-      <c r="D70" s="68"/>
+      <c r="B70" s="74"/>
+      <c r="C70" s="74"/>
+      <c r="D70" s="74"/>
       <c r="E70" s="23">
         <v>10</v>
       </c>
@@ -2023,12 +2354,12 @@
       </c>
     </row>
     <row r="71" spans="1:7">
-      <c r="A71" s="58" t="s">
+      <c r="A71" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="B71" s="58"/>
-      <c r="C71" s="58"/>
-      <c r="D71" s="58"/>
+      <c r="B71" s="75"/>
+      <c r="C71" s="75"/>
+      <c r="D71" s="75"/>
       <c r="E71" s="23">
         <v>20</v>
       </c>
@@ -2037,12 +2368,12 @@
       </c>
     </row>
     <row r="72" spans="1:7">
-      <c r="A72" s="58" t="s">
+      <c r="A72" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="B72" s="58"/>
-      <c r="C72" s="58"/>
-      <c r="D72" s="58"/>
+      <c r="B72" s="75"/>
+      <c r="C72" s="75"/>
+      <c r="D72" s="75"/>
       <c r="E72" s="23">
         <v>10</v>
       </c>
@@ -2051,12 +2382,12 @@
       </c>
     </row>
     <row r="73" spans="1:7">
-      <c r="A73" s="68" t="s">
+      <c r="A73" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="B73" s="68"/>
-      <c r="C73" s="68"/>
-      <c r="D73" s="68"/>
+      <c r="B73" s="74"/>
+      <c r="C73" s="74"/>
+      <c r="D73" s="74"/>
       <c r="E73" s="23">
         <v>20</v>
       </c>
@@ -2065,12 +2396,12 @@
       </c>
     </row>
     <row r="74" spans="1:7">
-      <c r="A74" s="68" t="s">
+      <c r="A74" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="B74" s="68"/>
-      <c r="C74" s="68"/>
-      <c r="D74" s="68"/>
+      <c r="B74" s="74"/>
+      <c r="C74" s="74"/>
+      <c r="D74" s="74"/>
       <c r="E74" s="23">
         <v>15</v>
       </c>
@@ -2079,12 +2410,12 @@
       </c>
     </row>
     <row r="75" spans="1:7">
-      <c r="A75" s="68" t="s">
+      <c r="A75" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="B75" s="68"/>
-      <c r="C75" s="68"/>
-      <c r="D75" s="68"/>
+      <c r="B75" s="74"/>
+      <c r="C75" s="74"/>
+      <c r="D75" s="74"/>
       <c r="E75" s="23">
         <v>10</v>
       </c>
@@ -2093,12 +2424,12 @@
       </c>
     </row>
     <row r="76" spans="1:7">
-      <c r="A76" s="58" t="s">
+      <c r="A76" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="B76" s="58"/>
-      <c r="C76" s="58"/>
-      <c r="D76" s="58"/>
+      <c r="B76" s="75"/>
+      <c r="C76" s="75"/>
+      <c r="D76" s="75"/>
       <c r="E76" s="23">
         <v>5</v>
       </c>
@@ -2107,12 +2438,12 @@
       </c>
     </row>
     <row r="77" spans="1:7">
-      <c r="A77" s="67" t="s">
+      <c r="A77" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="B77" s="67"/>
-      <c r="C77" s="67"/>
-      <c r="D77" s="67"/>
+      <c r="B77" s="76"/>
+      <c r="C77" s="76"/>
+      <c r="D77" s="76"/>
       <c r="E77" s="23">
         <v>10</v>
       </c>
@@ -2121,12 +2452,12 @@
       </c>
     </row>
     <row r="78" spans="1:7">
-      <c r="A78" s="67" t="s">
-        <v>10</v>
-      </c>
-      <c r="B78" s="67"/>
-      <c r="C78" s="67"/>
-      <c r="D78" s="67"/>
+      <c r="A78" s="76" t="s">
+        <v>10</v>
+      </c>
+      <c r="B78" s="76"/>
+      <c r="C78" s="76"/>
+      <c r="D78" s="76"/>
       <c r="E78" s="23">
         <v>15</v>
       </c>
@@ -2135,12 +2466,12 @@
       </c>
     </row>
     <row r="79" spans="1:7">
-      <c r="A79" s="58" t="s">
+      <c r="A79" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="B79" s="58"/>
-      <c r="C79" s="58"/>
-      <c r="D79" s="58"/>
+      <c r="B79" s="75"/>
+      <c r="C79" s="75"/>
+      <c r="D79" s="75"/>
       <c r="E79" s="13">
         <v>5</v>
       </c>
@@ -2149,12 +2480,12 @@
       </c>
     </row>
     <row r="80" spans="1:7">
-      <c r="A80" s="58" t="s">
+      <c r="A80" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="B80" s="58"/>
-      <c r="C80" s="58"/>
-      <c r="D80" s="58"/>
+      <c r="B80" s="75"/>
+      <c r="C80" s="75"/>
+      <c r="D80" s="75"/>
       <c r="E80" s="13">
         <v>7</v>
       </c>
@@ -2247,14 +2578,14 @@
       </c>
     </row>
     <row r="89" spans="1:6">
-      <c r="A89" s="60" t="s">
+      <c r="A89" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="B89" s="60"/>
-      <c r="C89" s="60"/>
-      <c r="D89" s="60"/>
-      <c r="E89" s="60"/>
-      <c r="F89" s="60"/>
+      <c r="B89" s="62"/>
+      <c r="C89" s="62"/>
+      <c r="D89" s="62"/>
+      <c r="E89" s="62"/>
+      <c r="F89" s="62"/>
     </row>
     <row r="90" spans="1:6">
       <c r="A90" s="39" t="s">
@@ -2271,12 +2602,12 @@
       </c>
     </row>
     <row r="91" spans="1:6">
-      <c r="A91" s="68" t="s">
+      <c r="A91" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="B91" s="68"/>
-      <c r="C91" s="68"/>
-      <c r="D91" s="68"/>
+      <c r="B91" s="74"/>
+      <c r="C91" s="74"/>
+      <c r="D91" s="74"/>
       <c r="E91" s="23">
         <v>10</v>
       </c>
@@ -2285,120 +2616,120 @@
       </c>
     </row>
     <row r="92" spans="1:6">
-      <c r="A92" s="69" t="s">
+      <c r="A92" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="B92" s="69"/>
-      <c r="C92" s="69"/>
-      <c r="D92" s="69"/>
+      <c r="B92" s="77"/>
+      <c r="C92" s="77"/>
+      <c r="D92" s="77"/>
       <c r="E92" s="23">
         <v>10</v>
       </c>
       <c r="F92" s="13"/>
     </row>
     <row r="93" spans="1:6">
-      <c r="A93" s="69" t="s">
+      <c r="A93" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="B93" s="69"/>
-      <c r="C93" s="69"/>
-      <c r="D93" s="69"/>
+      <c r="B93" s="77"/>
+      <c r="C93" s="77"/>
+      <c r="D93" s="77"/>
       <c r="E93" s="23">
         <v>15</v>
       </c>
       <c r="F93" s="13"/>
     </row>
     <row r="94" spans="1:6">
-      <c r="A94" s="69" t="s">
+      <c r="A94" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="B94" s="69"/>
-      <c r="C94" s="69"/>
-      <c r="D94" s="69"/>
+      <c r="B94" s="77"/>
+      <c r="C94" s="77"/>
+      <c r="D94" s="77"/>
       <c r="E94" s="23">
         <v>12</v>
       </c>
       <c r="F94" s="13"/>
     </row>
     <row r="95" spans="1:6">
-      <c r="A95" s="58" t="s">
+      <c r="A95" s="75" t="s">
         <v>48</v>
       </c>
-      <c r="B95" s="58"/>
-      <c r="C95" s="58"/>
-      <c r="D95" s="58"/>
+      <c r="B95" s="75"/>
+      <c r="C95" s="75"/>
+      <c r="D95" s="75"/>
       <c r="E95" s="23">
         <v>8</v>
       </c>
       <c r="F95" s="13"/>
     </row>
     <row r="96" spans="1:6">
-      <c r="A96" s="58" t="s">
+      <c r="A96" s="75" t="s">
         <v>49</v>
       </c>
-      <c r="B96" s="58"/>
-      <c r="C96" s="58"/>
-      <c r="D96" s="58"/>
+      <c r="B96" s="75"/>
+      <c r="C96" s="75"/>
+      <c r="D96" s="75"/>
       <c r="E96" s="23">
         <v>4</v>
       </c>
       <c r="F96" s="13"/>
     </row>
     <row r="97" spans="1:6">
-      <c r="A97" s="69" t="s">
+      <c r="A97" s="77" t="s">
         <v>50</v>
       </c>
-      <c r="B97" s="69"/>
-      <c r="C97" s="69"/>
-      <c r="D97" s="69"/>
+      <c r="B97" s="77"/>
+      <c r="C97" s="77"/>
+      <c r="D97" s="77"/>
       <c r="E97" s="23">
         <v>7.5</v>
       </c>
       <c r="F97" s="13"/>
     </row>
     <row r="98" spans="1:6">
-      <c r="A98" s="69" t="s">
+      <c r="A98" s="77" t="s">
         <v>51</v>
       </c>
-      <c r="B98" s="69"/>
-      <c r="C98" s="69"/>
-      <c r="D98" s="69"/>
+      <c r="B98" s="77"/>
+      <c r="C98" s="77"/>
+      <c r="D98" s="77"/>
       <c r="E98" s="23">
         <v>6</v>
       </c>
       <c r="F98" s="13"/>
     </row>
     <row r="99" spans="1:6">
-      <c r="A99" s="58" t="s">
+      <c r="A99" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="B99" s="58"/>
-      <c r="C99" s="58"/>
-      <c r="D99" s="58"/>
+      <c r="B99" s="75"/>
+      <c r="C99" s="75"/>
+      <c r="D99" s="75"/>
       <c r="E99" s="23">
         <v>4</v>
       </c>
       <c r="F99" s="13"/>
     </row>
     <row r="100" spans="1:6">
-      <c r="A100" s="58" t="s">
+      <c r="A100" s="75" t="s">
         <v>53</v>
       </c>
-      <c r="B100" s="58"/>
-      <c r="C100" s="58"/>
-      <c r="D100" s="58"/>
+      <c r="B100" s="75"/>
+      <c r="C100" s="75"/>
+      <c r="D100" s="75"/>
       <c r="E100" s="23">
         <v>2</v>
       </c>
       <c r="F100" s="13"/>
     </row>
     <row r="101" spans="1:6">
-      <c r="A101" s="68" t="s">
+      <c r="A101" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="B101" s="68"/>
-      <c r="C101" s="68"/>
-      <c r="D101" s="68"/>
+      <c r="B101" s="74"/>
+      <c r="C101" s="74"/>
+      <c r="D101" s="74"/>
       <c r="E101" s="23">
         <v>20</v>
       </c>
@@ -2407,12 +2738,12 @@
       </c>
     </row>
     <row r="102" spans="1:6">
-      <c r="A102" s="68" t="s">
+      <c r="A102" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="B102" s="68"/>
-      <c r="C102" s="68"/>
-      <c r="D102" s="68"/>
+      <c r="B102" s="74"/>
+      <c r="C102" s="74"/>
+      <c r="D102" s="74"/>
       <c r="E102" s="23">
         <v>15</v>
       </c>
@@ -2421,12 +2752,12 @@
       </c>
     </row>
     <row r="103" spans="1:6">
-      <c r="A103" s="68" t="s">
+      <c r="A103" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="B103" s="68"/>
-      <c r="C103" s="68"/>
-      <c r="D103" s="68"/>
+      <c r="B103" s="74"/>
+      <c r="C103" s="74"/>
+      <c r="D103" s="74"/>
       <c r="E103" s="23">
         <v>10</v>
       </c>
@@ -2435,12 +2766,12 @@
       </c>
     </row>
     <row r="104" spans="1:6">
-      <c r="A104" s="58" t="s">
+      <c r="A104" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="B104" s="58"/>
-      <c r="C104" s="58"/>
-      <c r="D104" s="58"/>
+      <c r="B104" s="75"/>
+      <c r="C104" s="75"/>
+      <c r="D104" s="75"/>
       <c r="E104" s="23">
         <v>5</v>
       </c>
@@ -2449,12 +2780,12 @@
       </c>
     </row>
     <row r="105" spans="1:6">
-      <c r="A105" s="67" t="s">
+      <c r="A105" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="B105" s="67"/>
-      <c r="C105" s="67"/>
-      <c r="D105" s="67"/>
+      <c r="B105" s="76"/>
+      <c r="C105" s="76"/>
+      <c r="D105" s="76"/>
       <c r="E105" s="23">
         <v>10</v>
       </c>
@@ -2463,12 +2794,12 @@
       </c>
     </row>
     <row r="106" spans="1:6">
-      <c r="A106" s="67" t="s">
-        <v>10</v>
-      </c>
-      <c r="B106" s="67"/>
-      <c r="C106" s="67"/>
-      <c r="D106" s="67"/>
+      <c r="A106" s="76" t="s">
+        <v>10</v>
+      </c>
+      <c r="B106" s="76"/>
+      <c r="C106" s="76"/>
+      <c r="D106" s="76"/>
       <c r="E106" s="23">
         <v>15</v>
       </c>
@@ -2477,12 +2808,12 @@
       </c>
     </row>
     <row r="107" spans="1:6">
-      <c r="A107" s="58" t="s">
+      <c r="A107" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="B107" s="58"/>
-      <c r="C107" s="58"/>
-      <c r="D107" s="58"/>
+      <c r="B107" s="75"/>
+      <c r="C107" s="75"/>
+      <c r="D107" s="75"/>
       <c r="E107" s="13">
         <v>5</v>
       </c>
@@ -2491,12 +2822,12 @@
       </c>
     </row>
     <row r="108" spans="1:6">
-      <c r="A108" s="58" t="s">
+      <c r="A108" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="B108" s="58"/>
-      <c r="C108" s="58"/>
-      <c r="D108" s="58"/>
+      <c r="B108" s="75"/>
+      <c r="C108" s="75"/>
+      <c r="D108" s="75"/>
       <c r="E108" s="13">
         <v>7</v>
       </c>
@@ -2589,14 +2920,14 @@
       </c>
     </row>
     <row r="117" spans="1:6">
-      <c r="A117" s="60" t="s">
+      <c r="A117" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="B117" s="60"/>
-      <c r="C117" s="60"/>
-      <c r="D117" s="60"/>
-      <c r="E117" s="60"/>
-      <c r="F117" s="60"/>
+      <c r="B117" s="62"/>
+      <c r="C117" s="62"/>
+      <c r="D117" s="62"/>
+      <c r="E117" s="62"/>
+      <c r="F117" s="62"/>
     </row>
     <row r="118" spans="1:6">
       <c r="A118" s="39" t="s">
@@ -2613,12 +2944,12 @@
       </c>
     </row>
     <row r="119" spans="1:6">
-      <c r="A119" s="68" t="s">
+      <c r="A119" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="B119" s="68"/>
-      <c r="C119" s="68"/>
-      <c r="D119" s="68"/>
+      <c r="B119" s="74"/>
+      <c r="C119" s="74"/>
+      <c r="D119" s="74"/>
       <c r="E119" s="23">
         <v>10</v>
       </c>
@@ -2627,12 +2958,12 @@
       </c>
     </row>
     <row r="120" spans="1:6">
-      <c r="A120" s="58" t="s">
+      <c r="A120" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="B120" s="58"/>
-      <c r="C120" s="58"/>
-      <c r="D120" s="58"/>
+      <c r="B120" s="75"/>
+      <c r="C120" s="75"/>
+      <c r="D120" s="75"/>
       <c r="E120" s="23">
         <v>30</v>
       </c>
@@ -2641,12 +2972,12 @@
       </c>
     </row>
     <row r="121" spans="1:6">
-      <c r="A121" s="58" t="s">
+      <c r="A121" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="B121" s="58"/>
-      <c r="C121" s="58"/>
-      <c r="D121" s="58"/>
+      <c r="B121" s="75"/>
+      <c r="C121" s="75"/>
+      <c r="D121" s="75"/>
       <c r="E121" s="23">
         <v>15</v>
       </c>
@@ -2655,12 +2986,12 @@
       </c>
     </row>
     <row r="122" spans="1:6">
-      <c r="A122" s="68" t="s">
+      <c r="A122" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="B122" s="68"/>
-      <c r="C122" s="68"/>
-      <c r="D122" s="68"/>
+      <c r="B122" s="74"/>
+      <c r="C122" s="74"/>
+      <c r="D122" s="74"/>
       <c r="E122" s="23">
         <v>50</v>
       </c>
@@ -2669,12 +3000,12 @@
       </c>
     </row>
     <row r="123" spans="1:6">
-      <c r="A123" s="68" t="s">
+      <c r="A123" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="B123" s="68"/>
-      <c r="C123" s="68"/>
-      <c r="D123" s="68"/>
+      <c r="B123" s="74"/>
+      <c r="C123" s="74"/>
+      <c r="D123" s="74"/>
       <c r="E123" s="23">
         <v>10</v>
       </c>
@@ -2683,12 +3014,12 @@
       </c>
     </row>
     <row r="124" spans="1:6">
-      <c r="A124" s="68" t="s">
+      <c r="A124" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="B124" s="68"/>
-      <c r="C124" s="68"/>
-      <c r="D124" s="68"/>
+      <c r="B124" s="74"/>
+      <c r="C124" s="74"/>
+      <c r="D124" s="74"/>
       <c r="E124" s="23">
         <v>50</v>
       </c>
@@ -2697,12 +3028,12 @@
       </c>
     </row>
     <row r="125" spans="1:6">
-      <c r="A125" s="58" t="s">
+      <c r="A125" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="B125" s="58"/>
-      <c r="C125" s="58"/>
-      <c r="D125" s="58"/>
+      <c r="B125" s="75"/>
+      <c r="C125" s="75"/>
+      <c r="D125" s="75"/>
       <c r="E125" s="23">
         <v>5</v>
       </c>
@@ -2711,12 +3042,12 @@
       </c>
     </row>
     <row r="126" spans="1:6">
-      <c r="A126" s="67" t="s">
+      <c r="A126" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="B126" s="67"/>
-      <c r="C126" s="67"/>
-      <c r="D126" s="67"/>
+      <c r="B126" s="76"/>
+      <c r="C126" s="76"/>
+      <c r="D126" s="76"/>
       <c r="E126" s="23">
         <v>10</v>
       </c>
@@ -2725,12 +3056,12 @@
       </c>
     </row>
     <row r="127" spans="1:6">
-      <c r="A127" s="67" t="s">
-        <v>10</v>
-      </c>
-      <c r="B127" s="67"/>
-      <c r="C127" s="67"/>
-      <c r="D127" s="67"/>
+      <c r="A127" s="76" t="s">
+        <v>10</v>
+      </c>
+      <c r="B127" s="76"/>
+      <c r="C127" s="76"/>
+      <c r="D127" s="76"/>
       <c r="E127" s="23">
         <v>15</v>
       </c>
@@ -2739,12 +3070,12 @@
       </c>
     </row>
     <row r="128" spans="1:6">
-      <c r="A128" s="58" t="s">
+      <c r="A128" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="B128" s="58"/>
-      <c r="C128" s="58"/>
-      <c r="D128" s="58"/>
+      <c r="B128" s="75"/>
+      <c r="C128" s="75"/>
+      <c r="D128" s="75"/>
       <c r="E128" s="13">
         <v>5</v>
       </c>
@@ -2753,12 +3084,12 @@
       </c>
     </row>
     <row r="129" spans="1:6">
-      <c r="A129" s="58" t="s">
+      <c r="A129" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="B129" s="58"/>
-      <c r="C129" s="58"/>
-      <c r="D129" s="58"/>
+      <c r="B129" s="75"/>
+      <c r="C129" s="75"/>
+      <c r="D129" s="75"/>
       <c r="E129" s="13">
         <v>7</v>
       </c>
@@ -2851,14 +3182,14 @@
       </c>
     </row>
     <row r="138" spans="1:6">
-      <c r="A138" s="60" t="s">
+      <c r="A138" s="62" t="s">
         <v>55</v>
       </c>
-      <c r="B138" s="60"/>
-      <c r="C138" s="60"/>
-      <c r="D138" s="60"/>
-      <c r="E138" s="60"/>
-      <c r="F138" s="60"/>
+      <c r="B138" s="62"/>
+      <c r="C138" s="62"/>
+      <c r="D138" s="62"/>
+      <c r="E138" s="62"/>
+      <c r="F138" s="62"/>
     </row>
     <row r="139" spans="1:6">
       <c r="A139" s="39" t="s">
@@ -2875,12 +3206,12 @@
       </c>
     </row>
     <row r="140" spans="1:6">
-      <c r="A140" s="66" t="s">
+      <c r="A140" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="B140" s="66"/>
-      <c r="C140" s="66"/>
-      <c r="D140" s="66"/>
+      <c r="B140" s="79"/>
+      <c r="C140" s="79"/>
+      <c r="D140" s="79"/>
       <c r="E140" s="13">
         <v>10</v>
       </c>
@@ -2889,12 +3220,12 @@
       </c>
     </row>
     <row r="141" spans="1:6">
-      <c r="A141" s="58" t="s">
+      <c r="A141" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="B141" s="58"/>
-      <c r="C141" s="58"/>
-      <c r="D141" s="58"/>
+      <c r="B141" s="75"/>
+      <c r="C141" s="75"/>
+      <c r="D141" s="75"/>
       <c r="E141" s="13">
         <v>30</v>
       </c>
@@ -2903,12 +3234,12 @@
       </c>
     </row>
     <row r="142" spans="1:6">
-      <c r="A142" s="58" t="s">
+      <c r="A142" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="B142" s="58"/>
-      <c r="C142" s="58"/>
-      <c r="D142" s="58"/>
+      <c r="B142" s="75"/>
+      <c r="C142" s="75"/>
+      <c r="D142" s="75"/>
       <c r="E142" s="13">
         <v>15</v>
       </c>
@@ -2917,12 +3248,12 @@
       </c>
     </row>
     <row r="143" spans="1:6">
-      <c r="A143" s="66" t="s">
+      <c r="A143" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="B143" s="66"/>
-      <c r="C143" s="66"/>
-      <c r="D143" s="66"/>
+      <c r="B143" s="79"/>
+      <c r="C143" s="79"/>
+      <c r="D143" s="79"/>
       <c r="E143" s="13">
         <v>50</v>
       </c>
@@ -2931,12 +3262,12 @@
       </c>
     </row>
     <row r="144" spans="1:6">
-      <c r="A144" s="66" t="s">
+      <c r="A144" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="B144" s="66"/>
-      <c r="C144" s="66"/>
-      <c r="D144" s="66"/>
+      <c r="B144" s="79"/>
+      <c r="C144" s="79"/>
+      <c r="D144" s="79"/>
       <c r="E144" s="13">
         <v>30</v>
       </c>
@@ -2945,12 +3276,12 @@
       </c>
     </row>
     <row r="145" spans="1:6">
-      <c r="A145" s="66" t="s">
+      <c r="A145" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="B145" s="66"/>
-      <c r="C145" s="66"/>
-      <c r="D145" s="66"/>
+      <c r="B145" s="79"/>
+      <c r="C145" s="79"/>
+      <c r="D145" s="79"/>
       <c r="E145" s="13">
         <v>50</v>
       </c>
@@ -2959,12 +3290,12 @@
       </c>
     </row>
     <row r="146" spans="1:6">
-      <c r="A146" s="58" t="s">
+      <c r="A146" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="B146" s="58"/>
-      <c r="C146" s="58"/>
-      <c r="D146" s="58"/>
+      <c r="B146" s="75"/>
+      <c r="C146" s="75"/>
+      <c r="D146" s="75"/>
       <c r="E146" s="13">
         <v>10</v>
       </c>
@@ -2973,12 +3304,12 @@
       </c>
     </row>
     <row r="147" spans="1:6">
-      <c r="A147" s="59" t="s">
+      <c r="A147" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="B147" s="59"/>
-      <c r="C147" s="59"/>
-      <c r="D147" s="59"/>
+      <c r="B147" s="78"/>
+      <c r="C147" s="78"/>
+      <c r="D147" s="78"/>
       <c r="E147" s="13">
         <v>10</v>
       </c>
@@ -2987,12 +3318,12 @@
       </c>
     </row>
     <row r="148" spans="1:6">
-      <c r="A148" s="59" t="s">
-        <v>10</v>
-      </c>
-      <c r="B148" s="59"/>
-      <c r="C148" s="59"/>
-      <c r="D148" s="59"/>
+      <c r="A148" s="78" t="s">
+        <v>10</v>
+      </c>
+      <c r="B148" s="78"/>
+      <c r="C148" s="78"/>
+      <c r="D148" s="78"/>
       <c r="E148" s="13">
         <v>15</v>
       </c>
@@ -3001,60 +3332,60 @@
       </c>
     </row>
     <row r="149" spans="1:6">
-      <c r="A149" s="59" t="s">
+      <c r="A149" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="B149" s="59"/>
-      <c r="C149" s="59"/>
-      <c r="D149" s="59"/>
+      <c r="B149" s="78"/>
+      <c r="C149" s="78"/>
+      <c r="D149" s="78"/>
       <c r="E149" s="4">
         <v>5</v>
       </c>
       <c r="F149" s="13"/>
     </row>
     <row r="150" spans="1:6">
-      <c r="A150" s="59" t="s">
+      <c r="A150" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="B150" s="59"/>
-      <c r="C150" s="59"/>
-      <c r="D150" s="59"/>
+      <c r="B150" s="78"/>
+      <c r="C150" s="78"/>
+      <c r="D150" s="78"/>
       <c r="E150" s="4">
         <v>10</v>
       </c>
       <c r="F150" s="13"/>
     </row>
     <row r="151" spans="1:6">
-      <c r="A151" s="59" t="s">
+      <c r="A151" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="B151" s="59"/>
-      <c r="C151" s="59"/>
-      <c r="D151" s="59"/>
+      <c r="B151" s="78"/>
+      <c r="C151" s="78"/>
+      <c r="D151" s="78"/>
       <c r="E151" s="4">
         <v>10</v>
       </c>
       <c r="F151" s="13"/>
     </row>
     <row r="152" spans="1:6">
-      <c r="A152" s="59" t="s">
+      <c r="A152" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="B152" s="59"/>
-      <c r="C152" s="59"/>
-      <c r="D152" s="59"/>
+      <c r="B152" s="78"/>
+      <c r="C152" s="78"/>
+      <c r="D152" s="78"/>
       <c r="E152" s="4">
         <v>15</v>
       </c>
       <c r="F152" s="13"/>
     </row>
     <row r="153" spans="1:6">
-      <c r="A153" s="58" t="s">
+      <c r="A153" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="B153" s="58"/>
-      <c r="C153" s="58"/>
-      <c r="D153" s="58"/>
+      <c r="B153" s="75"/>
+      <c r="C153" s="75"/>
+      <c r="D153" s="75"/>
       <c r="E153" s="4">
         <v>5</v>
       </c>
@@ -3063,12 +3394,12 @@
       </c>
     </row>
     <row r="154" spans="1:6">
-      <c r="A154" s="58" t="s">
+      <c r="A154" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="B154" s="58"/>
-      <c r="C154" s="58"/>
-      <c r="D154" s="58"/>
+      <c r="B154" s="75"/>
+      <c r="C154" s="75"/>
+      <c r="D154" s="75"/>
       <c r="E154" s="4">
         <v>7</v>
       </c>
@@ -3161,94 +3492,36 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="111">
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A22:F22"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="A49:D49"/>
-    <mergeCell ref="A50:D50"/>
-    <mergeCell ref="A51:D51"/>
-    <mergeCell ref="F51:F52"/>
-    <mergeCell ref="A52:D52"/>
-    <mergeCell ref="A53:D53"/>
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A56:D56"/>
-    <mergeCell ref="A57:D57"/>
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="A62:D62"/>
-    <mergeCell ref="A64:D64"/>
-    <mergeCell ref="A65:D65"/>
-    <mergeCell ref="A68:F68"/>
-    <mergeCell ref="A70:D70"/>
-    <mergeCell ref="A71:D71"/>
-    <mergeCell ref="A72:D72"/>
-    <mergeCell ref="A73:D73"/>
-    <mergeCell ref="A74:D74"/>
-    <mergeCell ref="A75:D75"/>
-    <mergeCell ref="A76:D76"/>
-    <mergeCell ref="A77:D77"/>
-    <mergeCell ref="A78:D78"/>
-    <mergeCell ref="A79:D79"/>
-    <mergeCell ref="A80:D80"/>
-    <mergeCell ref="A89:F89"/>
-    <mergeCell ref="A91:D91"/>
-    <mergeCell ref="A92:D92"/>
-    <mergeCell ref="A93:D93"/>
-    <mergeCell ref="A94:D94"/>
-    <mergeCell ref="A95:D95"/>
-    <mergeCell ref="A148:D148"/>
-    <mergeCell ref="A149:D149"/>
-    <mergeCell ref="A123:D123"/>
-    <mergeCell ref="A124:D124"/>
-    <mergeCell ref="A125:D125"/>
-    <mergeCell ref="A126:D126"/>
-    <mergeCell ref="A127:D127"/>
-    <mergeCell ref="A128:D128"/>
-    <mergeCell ref="A129:D129"/>
-    <mergeCell ref="A138:F138"/>
-    <mergeCell ref="A140:D140"/>
-    <mergeCell ref="A106:D106"/>
-    <mergeCell ref="A107:D107"/>
-    <mergeCell ref="A108:D108"/>
-    <mergeCell ref="A117:F117"/>
-    <mergeCell ref="A119:D119"/>
-    <mergeCell ref="A120:D120"/>
-    <mergeCell ref="A121:D121"/>
-    <mergeCell ref="A122:D122"/>
-    <mergeCell ref="A96:D96"/>
-    <mergeCell ref="A97:D97"/>
-    <mergeCell ref="A98:D98"/>
-    <mergeCell ref="A99:D99"/>
-    <mergeCell ref="A100:D100"/>
-    <mergeCell ref="A101:D101"/>
-    <mergeCell ref="A102:D102"/>
-    <mergeCell ref="A103:D103"/>
-    <mergeCell ref="A104:D104"/>
+  <mergeCells count="140">
+    <mergeCell ref="P33:S33"/>
+    <mergeCell ref="P34:S34"/>
+    <mergeCell ref="P35:S35"/>
+    <mergeCell ref="P36:S36"/>
+    <mergeCell ref="P37:S37"/>
+    <mergeCell ref="P38:S38"/>
+    <mergeCell ref="P39:S39"/>
+    <mergeCell ref="J43:N43"/>
+    <mergeCell ref="J44:N44"/>
+    <mergeCell ref="P28:S28"/>
+    <mergeCell ref="P29:S29"/>
+    <mergeCell ref="P30:S30"/>
+    <mergeCell ref="P31:S31"/>
+    <mergeCell ref="P32:S32"/>
+    <mergeCell ref="N39:O39"/>
+    <mergeCell ref="J36:M36"/>
+    <mergeCell ref="J38:M38"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="N32:O32"/>
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="N34:O34"/>
+    <mergeCell ref="N35:O35"/>
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="N37:O37"/>
+    <mergeCell ref="N38:O38"/>
     <mergeCell ref="J22:M22"/>
     <mergeCell ref="A150:D150"/>
     <mergeCell ref="A151:D151"/>
@@ -3273,6 +3546,93 @@
     <mergeCell ref="A146:D146"/>
     <mergeCell ref="A147:D147"/>
     <mergeCell ref="A105:D105"/>
+    <mergeCell ref="A106:D106"/>
+    <mergeCell ref="A107:D107"/>
+    <mergeCell ref="A108:D108"/>
+    <mergeCell ref="A117:F117"/>
+    <mergeCell ref="A119:D119"/>
+    <mergeCell ref="A120:D120"/>
+    <mergeCell ref="A121:D121"/>
+    <mergeCell ref="A122:D122"/>
+    <mergeCell ref="A96:D96"/>
+    <mergeCell ref="A97:D97"/>
+    <mergeCell ref="A98:D98"/>
+    <mergeCell ref="A99:D99"/>
+    <mergeCell ref="A100:D100"/>
+    <mergeCell ref="A101:D101"/>
+    <mergeCell ref="A102:D102"/>
+    <mergeCell ref="A103:D103"/>
+    <mergeCell ref="A104:D104"/>
+    <mergeCell ref="A148:D148"/>
+    <mergeCell ref="A149:D149"/>
+    <mergeCell ref="A123:D123"/>
+    <mergeCell ref="A124:D124"/>
+    <mergeCell ref="A125:D125"/>
+    <mergeCell ref="A126:D126"/>
+    <mergeCell ref="A127:D127"/>
+    <mergeCell ref="A128:D128"/>
+    <mergeCell ref="A129:D129"/>
+    <mergeCell ref="A138:F138"/>
+    <mergeCell ref="A140:D140"/>
+    <mergeCell ref="A78:D78"/>
+    <mergeCell ref="A79:D79"/>
+    <mergeCell ref="A80:D80"/>
+    <mergeCell ref="A89:F89"/>
+    <mergeCell ref="A91:D91"/>
+    <mergeCell ref="A92:D92"/>
+    <mergeCell ref="A93:D93"/>
+    <mergeCell ref="A94:D94"/>
+    <mergeCell ref="A95:D95"/>
+    <mergeCell ref="A68:F68"/>
+    <mergeCell ref="A70:D70"/>
+    <mergeCell ref="A71:D71"/>
+    <mergeCell ref="A72:D72"/>
+    <mergeCell ref="A73:D73"/>
+    <mergeCell ref="A74:D74"/>
+    <mergeCell ref="A75:D75"/>
+    <mergeCell ref="A76:D76"/>
+    <mergeCell ref="A77:D77"/>
+    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A56:D56"/>
+    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="A62:D62"/>
+    <mergeCell ref="A64:D64"/>
+    <mergeCell ref="A65:D65"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="A50:D50"/>
+    <mergeCell ref="A51:D51"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="A52:D52"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:D11"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>